<commit_message>
Adiciona pré-processamento dos dados extraídos do arquivo bruto 'OMIEC'
</commit_message>
<xml_diff>
--- a/dataframes/OMIEC_RESPONSES.xlsx
+++ b/dataframes/OMIEC_RESPONSES.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Poly(thiophene-3-acetate-5-carboxylate); Poly(PTTA); PEDOT:PSS; Poly(3,4-ethylene-dioxythiophene) (PEDOT); Poly(3-hexylthiophene) (P3HT); Poly[2-methoxy-5-(3′-ethoxyphenyl)-ethoxy)-thiophene] (METH); Poly(3,4-propylenedioxythiophene) (PDOT); Poly(3,4-ethylenedioxythiophene) (EDOT); Poly(fluorene-co-benzothiadiazole) (PFBT); Poly-(3-butylthiophene)(PBUT); Poly[2,2'-bithiophene-5-carboxylic acid] (PBTCA); PT-PSS; Poly(thiophene) (PT); Poly(3,4-phenylenethiophene) (PPhT)</t>
+          <t>Polymer; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3,4-ethylenedioxylthiophene)/Poly(ethylene oxide) (PEDOT/PEO); Poly(3,4-ethylenedioxylthiophene)/Poly(spirobenzopyrane) (PEDOT/PSB);</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; PEDOT:PolyDADMA FSI; PEDOT:PolyDADMA TFSI; PEDOT:PolyDADMA Cl; PEDOT:PolyDADMA Tos; PEDOT:PolyDADMA FSI/[C2mpyr][FSI]; PEDOT:PolyDADMA X/[C2mpyr][X]</t>
+          <t>PEDOT:PSS; PEDOT:PolyDADMA FSI; PEDOT:PolyDADMA TFSI; PEDOT:PolyDADMA CF3SO3; PEDOT:PolyDADMA Tos; PEDOT:PolyDADMA FSI/[C(2)mpyr][FSI]</t>
         </is>
       </c>
     </row>
@@ -481,7 +481,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Polyvinylcarbazole; Poly(3,4-ethylenedioxythiophene); Polypyrrole; PEDOT-PSS; Poly(P-phenylie); PSS-Poly(3,4-ethylenedioxythiophene); Poly(dithiophene-co-azomethine); Poly(aniline-co-o-methylaniline); Poly(3,4-dialkoxy-2,5-thienylene); Poly(3,4-alkyloxy-2,5-thienylene); Poly(phenylene sulfide); Poly(3,4-ethylenedioxy-1,2-quinoline); Poly(o-methoxy, p-tolylamino-1,4-phenylene); Poly(phenyl-4',4"-diphenylacetylene); Poly(phenyl-2',5"-diethynyleneterephthalate); Poly(phenyl-1',3"-diethynyleneterephthalate); Poly(bithiophene-co-benzothiadiazole);</t>
+          <t>Conjugated Polymers; Poly(3,4-ethylenedioxythiophene); Poly(aniline-co-o-anisidine); Poly(thiophene); Poly(pyrrole-co-o-anisidine); Poly(phenylenevinylene); Poly(phenylene)s; Poly(p-phenylene vinylene)</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylene dioxythiophene)-poly(styrenesulfonate) (PEDOT:PSS); P3HT-PCBM (Poly(3-hexylthiophene)-[6,6]-Phenyl C61-butyric acid methyl ester); P(E-T)DT (Poly(2,6-(1,4)ethylenedioxy)-N,N'-bis(2-methyl)-P-phenylene vinylene); PTCDA (Poly(10,2-N,N-diheptadecanyl-2,9-endoethanoanthracene-2,3,4,5,6,7,8,9,10,11)-N,N-diheptadecanyl-2,9-endoethanoanthracene);</t>
+          <t>Organic synaptic diode</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>PEPDSeCI/PEDOT:PSS; PEMA-Konjac; PPy/P(NIPAm-co-MA); PEDOT-PSS; PSS-doped PEO; P(EPDM-co-MA); P(PEIE-co-EMA)</t>
+          <t>P3HT-PF6; PEDOT:PSS; poly(3,4-ethylene dioxythiophene) (PEDOT); Nafion-Poly(3,4-ethylene dioxythiophene) (PEDOT); poly(phenyl-enevinylene) (PPV); poly([2-methoxy-5-(3',7'-dimethyloctyloxy)-p-phenylenevinylene]) (MDMO-PPV); poly(N-alkylated-3,4-ethylene dioxythiophene); poly(2-methoxy-5-(3',7'-dimethyloctyl)-1,4-phenylenevinylene); PEDOT-Tosylate; Poly(ethylene oxide)/Poly(3,4-ethylenedioxythiophene) (PEO/PEDOT); Poly(vinyl benzyl chloride) (PVBC); Poly(phenylene alkyl side chain)/Poly(9-ethylcarbazole); Poly(phenylene alkyl side chain) (PPAS); Poly(3-hexylthiophene) (P3HT); Poly(3,3'-dioctyl-2,2'-bithiophene) (PDOOT); Poly(3,4-ethylenedioxythiophene)/Poly(3,4-ethylenedioxythiophene)/Polystyrene Sulphonate (PEDOT/PSS/PS);</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P3MT; PEDOT; PEDOT:PSS; PTh; PMMA; PPy; PTh-Methyl; PTh-PS; PTh-SO3H</t>
+          <t>Poly(N-vinylcarbazole); Poly(3,4-ethylenedioxythiophene); None</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) - Poly(styrenesulfonate); poly(neural networks); poly(triarylamine); poly(monoaza[18]crown-6)</t>
+          <t>PEDOT:PSS; PEO; Polythiophene; PEO:LiClO4; PEO:ZnCl2</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P3HT; Poly(3-hexylthiophene); Polythiophene derivatives</t>
+          <t>Polythiophene; poly(3-hexylthiophene)</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Polyaniline/poly(4-styrene sulfonic acid); Poly(3,4-ethylenedioxythiophene)/Poly(4-styrene sulfonic acid); Poly(3-hexylthiophene)/Poly(styrenesulfonate); Poly(thiophene-3-acetic acid)/Poly(4-styrene sulfonic acid)</t>
+          <t>PANI/PSS</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3,4-ethylenedioxythiophene)-Poly(4-styrenesulfonate) (PEDOT:PSS); Polyphenol; Polyphenylenevinylene; Polyfluorene; Polyaniline; Polythiophene</t>
+          <t>Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate) (PEDOT:PSS); Poly(3,4-ethylenedioxythiophene)-poly(3,4-ethylenedioxythiophene sulfonate) (PEDOT-PSS)</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Naphthodithiophene diimide-based polymer</t>
+          <t>naphthodithiophene diimide-based polymer</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-methylthiophene) (PMT); Poly(phenylene vinylene) (PPV); Poly(threne); Poly(triarylamine) (PTAA); Poly(2-Methoxy-5-(2'-Ethyl-Hexyloxy)-P-phenylene Vinylene) (MEH-PPV); Poly(2,5-Dimethoxy-1,4-phenylene Vinylene) (MDOPV); Poly(2,7-Carbazole-1,4-phenylene Vinylene) (CBPV); Poly(3,4,9,10-perylenetetracarboxylic di-imide-2,6-bis (ethyleneoxy) ethane) (PPEO);</t>
+          <t>P(NDI2OD-T2); P3HT; PTB7; PCEBT; PSU; P3T; PMBT; PEF; PEIZ; PVP.</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>PTAA-PEDOT; PCEI-PEDOT; TTF-TCNQ; EDOT-TTF; BEDT-TTF-PBr3; PSSH-TCP; PEP-PEDOT; PEDOT-TTF</t>
+          <t>N,N'-Bis(2,2,2-trifluoroethyl)-N,N'-bis(3-methylthiophen-2-yl)-benzidine; Poly(3,4-ethylenedioxythiophene); PEDOT-PSS; Poly(3-hexylthiophene); Poly(thieno[3,4-b]thiophene); Naphthalenediimide-Functionalized Polymers</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)/poly(4-styrenesulfonate)</t>
+          <t>Poly(3,4-ethylenedioxythiophene)/poly(4-styrenesulfonate);</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>PEDOT; EDOTS-EDOTCOOH copolymers</t>
+          <t>PEDOT-EDOTS; PEDOT-EDOTCOOH</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>poly(3,4-ethylenedioxythiophene):poly(styrenesulfonic acid);</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P3HT;</t>
+          <t>P3HT</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Polymer Electrolyte Complex (PEC); Poly(ethylene oxide)-Li salts (PEO-Li salts); Poly(methylmethacrylate)-ZnPhen (PMMA-ZnPhen); Poly(vinylidene fluoride)-Li salts (PVDF-Li salts); Poly(vinylene carbonate)-Li salts (PVC-Li salts); Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate) (PEDOT-PSS)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>PEDOT-PSS; PEO-LiClO4; PBI-H3PO4; P3HT-LiClO4</t>
+          <t>Polymer; Ion gel-electrolyte</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>PEG-DMEA; PIMA; PIIF; PTAA; DPP-DTB; DPP-DCA; PBDT-TT; F4TCN-Q; PTPA; PFEDOT; PBTT-TT; PBDT-BT; PTTS; TTF-Th; P4P; PFO-DPS; DPP-BT; PCEI; TTT-T.</t>
+          <t>PEDOT:PSS; PPV; P3HT; PTMM; PFOBT; PThP; PEO; PEM; PECPP; PFO; P4V; PPE; POMe; PMEG; PBTTT; P3AT; PEO-PTFE; POPOP; PBI; PP; PFCB</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>PEDOT-PSS; poly[2-methoxy-5-(2-ethylhexyloxy)-1,4-phenylenevinylene]-block-polyethylene glycol; None</t>
+          <t>Polymerethane-glycols; Polyfluorene-ethyleneglycol; Polythiophene-ethyleneglycol</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>PEDOTP; PSS-PEDOT; Poly(aniline-co-o-toluidine); Poly(ethylene dioxythiophene):Poly(ethylene oxide); Poly(phenylene vinylene)</t>
+          <t>Polymer film;</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,8 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Polyvinylcarbazole; π-conjugated oligoaniline; Phenyl-C61-butyracid methyl ester (PCBM)</t>
+          <t>Polymer materials mentioned in the text are:
+Polyparaphenylene vinylene;</t>
         </is>
       </c>
     </row>
@@ -761,7 +762,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>AN-based polymers; naphthalene-π-conjugated polymers</t>
+          <t>AN-based polymers</t>
         </is>
       </c>
     </row>
@@ -771,7 +772,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Dan-Pffee-PPV; Poly(3,4-ethylenedioxythiophene); Poly(9,9-dioctylfluorene-alt-5,5-(4,7-di-2-thienyl)-2,1,3-benzothiadiazole)</t>
+          <t>P3HT; PANI; PSSA</t>
         </is>
       </c>
     </row>
@@ -781,7 +782,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Ni-3(HITP)(2)</t>
+          <t>Ni-3(hexaiminotriphenylene)(2);</t>
         </is>
       </c>
     </row>
@@ -811,7 +812,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>gNR-Bu;</t>
+          <t>poly(gNR-Bu);</t>
         </is>
       </c>
     </row>
@@ -821,7 +822,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3,4-ethylenedioxythiophene)-co-poly(styrenesulfonate); Polyvinylferrocene; Poly(phenylenevinylene) (PPV); Poly(3-hexylthiophene) (P3HT); Poly(p-phenyleneethynylene) (PPE); Poly(2-methoxy-5-(2'-ethylhexyloxy)-p-phenylenevinylene) (MEH-PPV); Poly(9,9-dioctylfluorene) (PFO); Poly[2-methoxy-5-(3',7'-dimethyloctyloxy)-p-phenylenevinylene];</t>
+          <t>PEN-TRIS; MEH-TRIS; PSS; PEDOT; P3HT; PFO; PPy; PBTTT; PTP-Et; PTTT; PAN;</t>
         </is>
       </c>
     </row>
@@ -831,7 +832,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; PEDOT:PDADMA-TFSI</t>
+          <t>PPSS; PPTFSI</t>
         </is>
       </c>
     </row>
@@ -851,7 +852,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Polymer; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(fluorene-phenylene-vinylene) (PPFV); Ned; Poly(phenylene-co-2,5-dioctoxy-p-phenylene vinylene) (PPV); Poly(3-alkylthiophene) (P3AT); Poly(spirofluorene-phenylene-vinylene) (PSFV); Poly(3,4-dialkoxy-2,5-thienylenevinylene) (PDOO-TVV); Poly(4-methyl-2,2-dioctyl-sebacate) (P4MS); Conjugated polymer; Poly(2,5-bis(3-t-butyl-2-carbonylthiophen-5-yl)-1,3,4-thiadiazole) (PBTS); Poly(3-alkoxy-4-methoxythiophene) (P3AXT); Poly(2-methoxy-5-(2-ethylhexyloxy)-p-phenylenevinylene) (MEH-PPV); Poly(3,4-ethylene-dioxythiophene)-poly(4-styrenesulfonate) (PEDOT-PSS).</t>
+          <t>Polymer-based electrolyte-TTF; P3HT-PSS; PEDOT:PSS; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-butyl-thiophene) (P3BTh);</t>
         </is>
       </c>
     </row>
@@ -861,7 +862,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Poly(3-butylthiophene-co-3-hexylthiophene), P3HT; conjugated polymer of silole; poly(3,4-ethylenedioxythiophene) (PEDOT)-poly(4-styrenesulfonate) (PSS); poly(3,4-ethylenedioxythiophene) (PEDOT)-poly(3-methylthiophene) (P3MT); poly(3-octylthiophene) (POTP); poly(vinyl-triethylene-tetrafluoroethylene) (PVTF); poly(N-alkylpyrrole); Poly(p-phenylene-ethynylene); poly(p-phenylene-vinylene); MeH-PPV; Derivatives of poly(phenylene-vinylene); Poly(3,4-propylenedioxythiophene); Poly(3,4-butyl-1,3,4-oxadiazol); Poly(3,4-ethyl-1,3,4-oxadiazol);</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -871,7 +872,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>NDI-T2;</t>
+          <t>NDI-T2 copolymers</t>
         </is>
       </c>
     </row>
@@ -891,7 +892,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Polymer;DOPV-OMMEC;P3HT:C60;PTAA-PSSA;PTAA-PFSA;PEO-PFSA;PEO-PFSA-DMA;PEDOT-PSSA;PEDOT-PFSA;PANI-PSSA;PANI-PFSA</t>
+          <t>Polymethylsilesquioxane-functionalized polythiophene; poly(3,4-ethylenedioxythiophene)-block-poly(ethylene oxide); poly(3,4-ethylenedioxythiophene)-block-poly(styrenesulfonate); conjugated polyelectrolyte; poly(thiophene-alt-anthraquinone); poly(3,4-ethylenedioxythiophene)-block-poly(caprolactone)</t>
         </is>
       </c>
     </row>
@@ -901,7 +902,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Polythiophene with tetraethylene glycol side chains; Carboxymethylated cellulose nanofibrils</t>
+          <t>Polythiophene with tetraethylene glycol side chains</t>
         </is>
       </c>
     </row>
@@ -911,8 +912,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Poly[di-2-pyridylamine-4,4'-bipyridine]
-Poly(ethylene oxide-bisphenol-A-carbonate) (PEO-PBA)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -922,7 +922,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>PAAM/PDA; PANI</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -932,7 +932,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>PolymerPV5T-F2T; polymerPV5T; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(2-methoxy-5-(2'-ethylhexyloxy)-p-phenylenevinylene) (MEH-PPV); Poly(dibenzo[a, c]phenazine-6,11-diyl); Poly(fluorene-co-bithiophene); Poly[2-methoxy-5-(2-ethylhexoxy)-1,4-phenylenevinylene] (MEH-PPV); Poly[3-alkylthiophene]; Poly(3-alkoxy-4-alkylthiophene)</t>
+          <t>PMDT-TPD; PIM-DT; PIM-TSTP; PTTP; PSETP; BIS-TTF; BEH-TTF</t>
         </is>
       </c>
     </row>
@@ -942,7 +942,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>PVA/PEDOT:PSS</t>
+          <t>PEDOT:PSS; none</t>
         </is>
       </c>
     </row>
@@ -952,7 +952,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Nanoseed-F; PEDOT-PSS; P3HT; F8T2; PFFT; PTTCNQ; DMFu; NiDBT; CoDBT; BCP-MeE; F4TCNQ; BDT-Th; TiPT-T; CoPc-T; PM6; PTMS; DBT-T; NDI-T; BDT-BT; DBT-BA; BDT-Cy; DNT-DP; BDT-MeE; NDI-MeE; DBT-P; BDT-P;</t>
+          <t>Polymer-modulated surface; Poly(ester) matrix; Poly(phenylenevinylene); Poly(3,4-ethylenedioxythiophene); Poly{[9,9-bis(6'-N-carbazolyl)fluorene]-2,7-diyl};</t>
         </is>
       </c>
     </row>
@@ -962,7 +962,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>poly(methyl-phenyl-silane); poly(vinyl-benzaldehyde); poly(phenyl-ethynyl-thiophene); None</t>
+          <t>Polymer; Poly(3,4-ethylenedioxythiophene) (PEDOT); PEDOT:Poly(styrenesulfonate) (PEDOT:PSS); Poly(3-methylthiophene);</t>
         </is>
       </c>
     </row>
@@ -972,7 +972,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P3HT-BT-FBBT; PTTP; PSI-DTTP; PSI-PTTP; PSI-DTTP-KY-Type; PSI-BT-Type</t>
+          <t>Polymer electrolyte; Poly[3,4-ethylenedioxythiophene] LiTFSI; Poly(thiophenehexafluorophosphate) Li+</t>
         </is>
       </c>
     </row>
@@ -982,7 +982,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>PEDOT:PSS; P3HT;</t>
         </is>
       </c>
     </row>
@@ -1012,7 +1012,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>PEDOT/PSS; Co-PEG-PEDOT; MEL121; PSS/PEO-PEDOT; ionic-fluorenyl-PEO; PEDOT-TMA; Nafion-PEDOT; polyaniline-PEDOT; Nafion; doped-PEDOT-PSS; PEO-PEDOT-PSS; conducting polymers; ionomeric polymers; fluorinated polymers; polylimides</t>
+          <t>Polymer/polymer names: Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(phenylene vinylene) (PPV); Poly(thiophene-3-alkylacetates) (PTA); Poly(3-methylthiophene) (PMT); Poly(o-phenylene-co-2,5-thienylene) (PPP-T); Poly(2-methoxy-5-(2-ethylhexyloxy)-p-phenylene vinylene) (MEHPPV)</t>
         </is>
       </c>
     </row>
@@ -1032,7 +1032,10 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>4-hydroxy TEMPO, HT; HT/LT/FT mixture</t>
+          <t>HT; T }}&lt;/assistant&lt;|end_header_id|&gt;
+I assume you meant to terminate the input text there.
+Here are the OMIEC polymers found:
+HT; F4TCNQ</t>
         </is>
       </c>
     </row>
@@ -1042,7 +1045,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>PEDOT/PSS</t>
+          <t>Pedot/PSS</t>
         </is>
       </c>
     </row>
@@ -1062,7 +1065,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Nonactin</t>
+          <t>nonactin</t>
         </is>
       </c>
     </row>
@@ -1072,7 +1075,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Polymer PEo-polyaniline; Polymer PEO-Bi2S3</t>
+          <t>Polyaniline;</t>
         </is>
       </c>
     </row>
@@ -1082,7 +1085,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>(PDMA)PbI4; (BzA)2PbI4; PDMA; BzA</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1092,7 +1095,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Polymer; PEDOT:PSS; PTh:PSS; P3HT:PSS; PPy:PSS</t>
+          <t>Poly(3,4-ethylenedioxythiophene); poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); None</t>
         </is>
       </c>
     </row>
@@ -1102,7 +1105,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>PNDI</t>
+          <t>PNDI;</t>
         </is>
       </c>
     </row>
@@ -1112,7 +1115,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>TTF-CA</t>
+          <t>TTF-CA;</t>
         </is>
       </c>
     </row>
@@ -1152,7 +1155,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>gNR; hgNR</t>
         </is>
       </c>
     </row>
@@ -1162,7 +1165,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Poly-(3,4-ethylenedioxythiophene)-benzoyl-(2-ethylhexyl)phosphonate (PEDOT-BEP); Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(9,9-dioctylfluorene-alt-benzothiadiazole) (F8BT); Poly(3-(2-methoxyethoxy)ethyl-9-carbazovinylene) (EMEV); Poly(3-phenylthiophene) (P3PT); Polyquinoline; Polyindole; PPy-PES; POMe-OMe; PEOEM; Poly[2-methoxy-5-(2-ethylhexyloxy)-p-phenylene vinylene] (MEH-PPV); Poly(3-butylthiophene) (PBT); Poly(3-heptylthiophene) (PHT); Poly[2-(2-ethylhexyloxy)-5-methoxy-p-phenylene vinylene] (EHO-MeOPPV); Poly(3-octylthiophene) (POT); Poly(3-nonylthiophene) (PNT); Poly(3-dodecylthiophene) (PDT); Poly(3-pentadecylthiophene) (PPT); Poly(3-hexadecylthiophene) (PHT);</t>
+          <t>Poly(3,4-ethylenedioxthiophene); Poly(aniline-co-o-ethyaniline); None</t>
         </is>
       </c>
     </row>
@@ -1182,7 +1185,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>p(N-T); poly(styrene); None</t>
+          <t>p(N-T); Polystyrene</t>
         </is>
       </c>
     </row>
@@ -1192,7 +1195,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>PEDOT: PSS;</t>
+          <t>PEDOT: PSS</t>
         </is>
       </c>
     </row>
@@ -1232,7 +1235,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Pymo; PEI-TPPY; PTAPP-PMIDA; PTA-PPh3; PTSA-DMF; PTP-TBAPP; PTPA-TTF; [PdII(pmepe)Cl2]; [PdII(bpy)Cl2]; [CuII(bpy)Cl2]; [ZnII(dpa)Cl2]; BDPA-BTBP; BDPA-P2N; BTBP-PTE; BDM-Based POM.</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1242,7 +1245,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-methylthiophene) (PMET); Poly(p-phenylene vinylene) (PPV); Poly(tetraphenylethene) (PTPE); Poly(9,9-dioctylfluorene) (PFO)</t>
+          <t>PvTP; PPy-HMT; PPy-PEI; PPy-MT; PANI; PEDOT-PSS; PThCl; P3HT; PEO-LiClO4; PANI-EDOT</t>
         </is>
       </c>
     </row>
@@ -1252,7 +1255,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>P3HT; PEDOT:PSS; Polyaniline; Poly(3,4-ethylenedioxythiophene)</t>
+          <t>Polymer materials: Poly(3,4-ethylenedioxythiophene);</t>
         </is>
       </c>
     </row>
@@ -1262,7 +1265,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Pedot</t>
+          <t>PEDOT;</t>
         </is>
       </c>
     </row>
@@ -1312,7 +1315,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>poly[norbornene-1,2bis(C(O)OPEDOT)]-b-[norbornene-1,2-bis-(C(O)PEG(12))];</t>
+          <t>PEDOT-b-PEG</t>
         </is>
       </c>
     </row>
@@ -1322,7 +1325,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>P-XO (X = 3-6)</t>
+          <t>P-3O; P-4O; P-5O; P-6O</t>
         </is>
       </c>
     </row>
@@ -1332,7 +1335,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(o-phenylenediamine); Poly(phenylene vinylene) (PPV); Poly(2-methoxy-5-(2'-ethylhexyloxy)-1,4-phenylenevinylene) (MEH-PPV)</t>
+          <t>Polymer;Poly(3,4-ethylenedioxythiophene) (PEDOT);Poly-(vinylladenyi fluoride) (PVDF);Polyurethane;Polyvinyl chloride (PVC)</t>
         </is>
       </c>
     </row>
@@ -1342,7 +1345,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Polyaniline (PANI); Poly(3,4-ethylenedioxythiophene-co-3-methylthiophene) (PEDOT:PSS); Poly(acrylic acid) (PAA); Poly(vinylidine fluoride) (PVDF); Poly(ethylene oxide) (PEO)</t>
+          <t>Polymer Nanostructured Pseudocapacitive PEDOT; Poly(3,4-ethylenedioxythiophene); Poly(3,4-ethylenedioxythiophene)/Polystyrene Sulfonate (PEDOT/PSS); Polythiophene; Poly(2-methoxy-5-(2'-ethylhexyloxy)-p-phenylenevinylene); Poly(phenylene vinylene); Poly(2-methoxy-5-(3',7'-dimethyloctyloxy)-p-phenylenevinylene)</t>
         </is>
       </c>
     </row>
@@ -1352,7 +1355,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>P3MEEET;</t>
+          <t>P3MEEET</t>
         </is>
       </c>
     </row>
@@ -1362,7 +1365,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>poly(3-hexylthiophene)</t>
+          <t>poly(3-hexylthiophene); lithium bis(trifluoromethanesulfonyl) imide (LiTFSI); dimethoxyethane (DME)</t>
         </is>
       </c>
     </row>
@@ -1372,7 +1375,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>PEDOT:PSS</t>
+          <t>PEDOT:PSS;</t>
         </is>
       </c>
     </row>
@@ -1392,7 +1395,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>bgTNR</t>
+          <t>TNR; bgTNR</t>
         </is>
       </c>
     </row>
@@ -1402,7 +1405,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Polyethylene dioxythiophene; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-hexylthiophene) (P3HT)</t>
+          <t>Polymer; Poly(3,4-ethylenedioxythiophene);</t>
         </is>
       </c>
     </row>
@@ -1422,7 +1425,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; Poly(3,4-ethylenedioxthiophene)-polystyrenesulfonate; Poly(3-hexylthiophene)-[6,6]-phenyl-C61-butyric acid methyl ester; PEO-based OMIECs; Poly(3,4-ethylenedioxthiophene)-[6,6]-phenyl-C61-butyric acid methyl ester; Polyaniline-poly(ethylene oxide); Poly(3-Octylthiophene)-poly(styrenesulfonate); None</t>
+          <t>Conjugated Polyelectrolyte; PEDOT:PSS; PEM; Poly(3,4-ethylenedioxythiophene)-block-Poly(ethylene oxide); PEDOT-PSS; PEDOT-PEO</t>
         </is>
       </c>
     </row>
@@ -1442,7 +1445,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>rr-P3HT;</t>
         </is>
       </c>
     </row>
@@ -1452,7 +1455,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Poly(p-phenylenevinylene)-Coated Poly(3,4-ethylenedioxythiophene); Poly(3,4-ethylenedioxythiophene)-Doped Poly(3-hydroxybutyrate-co-3-hydroxyvalerate); None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1482,7 +1485,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Polymer; PTh-TEG; PTh-TS; PPy-Fluorine; P3HT-Fluorine</t>
+          <t>Polymer systems</t>
         </is>
       </c>
     </row>
@@ -1492,7 +1495,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>NDIP</t>
+          <t>NDIP;</t>
         </is>
       </c>
     </row>
@@ -1512,7 +1515,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>PolyNEDIMethylpentacene; Poly(3,4-ethylenedioxythiophene); Poly(diallyldimethylammonium chloride); Poly(2-methoxy-5-(2-ethylhexyloxy)-1,4-phenylenevinylene)</t>
+          <t>PEDOT:PSS; PBTTT; Pppy; P3HT; PFO; PPE-TT; F4TFBT; TTF-based OMIECs</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1525,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>PEDOT:Tos</t>
+          <t>poly(3,4-ethylenedioxythiophene):tosylate (PEDOT:Tos)</t>
         </is>
       </c>
     </row>
@@ -1532,7 +1535,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Polypyrrole-polyaniline; Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); Poly(3-hexylthiophene)-poly(styrenesulfonate)</t>
+          <t>Poly(3,4-ethylenedioxythiophene)-[poly(4-styrenesulfonate)], Poly(N-methylated poly(phenylene sulfide));</t>
         </is>
       </c>
     </row>
@@ -1542,7 +1545,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); Poly(fluorene-co-benzothiadiazole); Poly(3-hexylthiophene)-poly(ethylene oxide);</t>
+          <t>Poly(N-alkyl-3,4-propylenedioxaniline); Poly(3,4-ethylenedioxypyrrolidone); Poly(dialkoxynaphthalene);</t>
         </is>
       </c>
     </row>
@@ -1572,7 +1575,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Polymer; Poly(3,4-ethylenedioxythiophene)-poly(4-styrenesulfonate); poly(vinylferrocene); Poly(phenylenevinylene); Poly(p-phenylene sulfide)</t>
+          <t>PEDOT-PSS; Poly(3,4-ethylenedioxythiophene); Poly(3-methylthiophene); Poly(3-hexylthiophene)</t>
         </is>
       </c>
     </row>
@@ -1582,7 +1585,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Poly(indigosol); Poly(indigo-methylene-isoindigo); Poly(indigo-methoxy-isoindigo)</t>
+          <t>polyisoindigo; polyisoindigo derivatives</t>
         </is>
       </c>
     </row>
@@ -1592,7 +1595,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Conjugated polymer electrodes; π-CNT/Poly(styrenesulfonate); PEDOT:PSS; Polyaniline-co-Dodecylbenzenesulfonate; Poly(3,4-ethylenedioxythiophene): poly(4-styrenesulfonate); Poly(vinylidene fluoride)-silicone; Poly(ethylenedioxythiophene): poly(ethylenedioxythiophene);</t>
+          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-methylthiophene) (P3MT); Poly(3-hexylthiophene) (P3HT)</t>
         </is>
       </c>
     </row>
@@ -1622,7 +1625,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>(BEDT-TTF)(Me,TCNQ); (BEDT-TTF)(CIMeTCNQ); (BEDO-TTF)(Cl(2)TCNQ)</t>
+          <t>(BEDO-TTF)(CI,TCNQ)</t>
         </is>
       </c>
     </row>
@@ -1632,7 +1635,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Poly(p-phenylene vinylene):PPV-alkyl sulfonate; Poly(3,4-ethylenedioxythiophene):PEDOT-undecylsulfonate; Poly(3-hexylthiophene):P3HT-hexanoate</t>
+          <t>Polymer; PEDOT-PSS; Poly(3,4-Ethylenedioxythiophene)/Poly(styrenesulfonate)</t>
         </is>
       </c>
     </row>
@@ -1642,7 +1645,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>PMA; P18; P28</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1652,7 +1655,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-hexylthiophene) (P3HT); Co-polymer of aniline and fluoraniline (EPA); Poly(phenylene vinylene) (PPV); Poly(aniline) (Pani); Polyaniline-based copolymer; Poly(3-butylthiophene) (PBTh); Poly(3-octylthiophene) (POTh)</t>
+          <t>PSS-PECDA; P3HT-Br; PEDOT-PSS; PBTTT-C12; PCE; PTCA; PTCDA; PTP; PISN-HMT; PISN-HTMS</t>
         </is>
       </c>
     </row>
@@ -1662,7 +1665,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>P3HT-IM</t>
+          <t>poly{3-[6'-(N-methylimidazolium)hexyl]thiophene}BF4- (P3HT-IM);</t>
         </is>
       </c>
     </row>
@@ -1702,7 +1705,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>( BEDO-TTF)Cl(2)TCNQ; (BEDT-TTF)ClMeTCNQ</t>
         </is>
       </c>
     </row>
@@ -1722,7 +1725,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>polymer;polythiophene;poly(ethylene glycol)</t>
+          <t>oligo(ethylene glycol) substituted regioregular polythiophene</t>
         </is>
       </c>
     </row>
@@ -1732,7 +1735,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>mLPPP; HMWPEO</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1745,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Poly(benzimidazophenothiazine); Poly(phenanthroline); Poly(phenothiazine); Poly(pyridine); Poly(quinoline); Poly(thieno[3,4-b]thiophene);</t>
+          <t>ethylene glycol functionalized conjugated polymers</t>
         </is>
       </c>
     </row>
@@ -1752,7 +1755,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>d-gdiPDI; naphthalene bis-isatin-based oligomers; isoindigo-based polymers; lactone-based conjugated polymers; naphthalene tetracarboxylic diimide copolymers</t>
+          <t>PDI-based d-gdiPDI; naphthalene bis-isatin based fused n-type small molecules; isoindigo-based polymers; lactone-based conjugated polymers; Naphthalene tetracarboxylic diimide copolymers</t>
         </is>
       </c>
     </row>
@@ -1762,7 +1765,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Polyvinylphenol-EDOT; Pyrrole-TiO2; PEDOT-grafted-polyglycerol; PEDOT-grafted-polysaccharides; Pyrrole-glycidylmethacrylate-polystyrene; PEDOT-g-C3N4; Conjugated polyaniline-Pd nanowires; PEDOT-g-PEG; PEDOT-grafted-PCL; Conductive poly(phenylene vinylene)-PVA; PEDOT-g-PCL; Poly(3,4-ethylenedioxythiophene)-g-PEG; Polyquaternium-4; Conjugated polyaniline-Ag nanowires; PEDOT-grafted-polycaprolactone; PEDOT-grafted-polyvinyl acetate; PEDOT-g-PLA; PEDOT-grafted-polylactic acid; PEDOT-g-PCL;</t>
+          <t>Polymer(s): Poly(3,4-ethylene dioxythiophene) (PEDOT); Poly(3,4-ethylene dioxythiophene)-Co-polystyrenesulfonate (PEDOT:PSS); Poly(dioxyaniline) (PANI); Poly(phenylene vinylene) (PPV)</t>
         </is>
       </c>
     </row>
@@ -1782,7 +1785,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>P3HT-gly; PPEV-gly; PFO-gly; P3HT-gly-alkyl; PPEV-gly-alkyl; PFm-TVT-gly-alkyl</t>
+          <t>Poly(3,4-ethylenedioxythiophene)-co-poly(styrenesulfonate); Poly(3,4-ethylenedioxythiophene)-co-poly(3-methylthiophene); None</t>
         </is>
       </c>
     </row>
@@ -1792,7 +1795,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Polythiophene (PT); poly(ethylene glycol) (PEG) side chains</t>
+          <t>Polythiophene (PT); polyethylene glycol (PEG); P1; P2; P3</t>
         </is>
       </c>
     </row>
@@ -1822,7 +1825,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>poly(3,4-ethylenedioxythiophene):poly(4-styrenesulfonate);</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -1832,7 +1835,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; P3HT; PANI; PBTTT; PDOT; PEF; PFN; PIVN; PPy; PTAA; PTCDI; PTTEIT; PTT; PVI; PVK; etc.</t>
+          <t>Poly(p-phenylene Vinylene); PSS-Ag; PEDOT; P3HT; PEI; PPy; PNiPAAm</t>
         </is>
       </c>
     </row>
@@ -1842,7 +1845,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; Poly(3,4-ethylenedioxythiophene)/Poly( styrenesulfonate); CooP3; PPy-MoS3; PEDOT/SWNT; P3HT:IM; P3T:IM; MEH-PPV:PCBM</t>
+          <t>PEDOT-MEL; P3HT-TFSI; P3HT-NTf2; Poly(phenylene ethynylene)-TFSI; Poly(phenylene vinylene)-NTf2</t>
         </is>
       </c>
     </row>
@@ -1862,7 +1865,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>PEDOT-PSS; PANI; PNPB; PBTTT; PEG; PMMA; P3HT; PFO; PPV</t>
+          <t>Conjugated Polymers; Mixed Conducting Polymer</t>
         </is>
       </c>
     </row>
@@ -1872,7 +1875,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>PEDOT:PSS</t>
+          <t>PEDOT:PSS;</t>
         </is>
       </c>
     </row>
@@ -1882,7 +1885,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Polymer-based OMIEC: TTF-CA</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1892,7 +1895,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>TTF-CA; PTCDI-PFMTDA; DPT-TBA; F16CuPc-F16CuPCC; NF-TTF; C60-PCBM; BIS-quinolinium-TCNQ; Cu-TCNQ; PVCN-PF6; F16CuPc-F16CuPCC-F16CuPCC; TTF-TCNQ; DNA-based OMIEC; μ-nitrophenyl-bis(ethylenedithio)tetrathiafulvalene; MEH-TCNQ</t>
+          <t>TTF-CA</t>
         </is>
       </c>
     </row>
@@ -1902,7 +1905,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Polypyrrole; Polyaniline; Poly(3,4-ethylenedioxythiophene) (PEDOT); Polyphenylene vinylene (PPV)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1912,7 +1915,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Polymer; MA(I)P (Methylammonium Lead Iodide); None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1942,7 +1945,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>PEDOT:PSS</t>
+          <t>PEDOT:PSS;</t>
         </is>
       </c>
     </row>
@@ -1952,7 +1955,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>PSSPT-TTBA; PEDOT-PSS; Poly(3-methyl-4-octylthiophene-co-3-methyl-4-octylthiophene-3-sulfonate); None</t>
+          <t>iAQMs;quinoidal para-azaquinodimethane (AQM)</t>
         </is>
       </c>
     </row>
@@ -1972,7 +1975,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>PBDTT-DPP; N,N'-Bis(2,5-di(thiophen-2-yl)phenyl)-N,N'-bis(2,5-di(thiophen-2-yl)phenyl)-1,6-benzothiazole-1,6-diium; TIPS-PEN-PTCDI; F16CuPc</t>
+          <t>PNDI-T2FBF-T2; P3HT-Se; PEO-LL; PMDECT-PPV; P3HT; PBTT; PTAA-Thiflu; P(SIPhiDT); PFO-DPP; PFDTBT; PFO-Pe4T; F8BT; F16CuPc; F3TCNQ; DMF-DPP; F8-BT; F8BiT; MeTPhF-BT; F3T; TTF-OMe; TTBA-Alcholine; TATA; TBTT; TFA-DPP.</t>
         </is>
       </c>
     </row>
@@ -1992,7 +1995,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Poly(N-vinylcarbazole)-imidazole; Poly(3,4-ethylenedioxythiophene)-polystyrene sulfonate; Poly(ethylene dioxythiophene)-polystyrene sulfonate; Poly(3-hexylthiophene)-perylene tetracarboxylic diimide; None</t>
+          <t>Polyparaphenylene ethynylene (PPE); Poly[2-methoxy-5-(2'-ethyl-hexyloxy)-p-phenylene vinylene] (MEH-PPV)</t>
         </is>
       </c>
     </row>
@@ -2012,7 +2015,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>(BEDT-TTF)(F(2)TCNQ); Unknown-3; Poly(3,4-ethylene dioxythiophene)-poly(styrenesulfonate) (PEDOT-PSS)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2022,7 +2025,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Poly[3-hydroxybenzaldehyde-2,6-di(2-thienyl)ethylene]; Poly(3,6-difluoro-7-methoxy-2,7-diaza-1-phosphabicyclo[2.2.2]oct-3-ene); none</t>
+          <t>PEDOT:PSS; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3,4-ethylenedioxythiophene): Poly(styrenesulfonate) (PEDOT:PSS); PBTTT-TTF; P3HT; Poly(3-hexylthiophene) (P3HT)</t>
         </is>
       </c>
     </row>
@@ -2032,7 +2035,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>BA; PEA; 1 T; 2P</t>
+          <t>BA+; PEA+; 1T+; 2P+</t>
         </is>
       </c>
     </row>
@@ -2042,7 +2045,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; Poly(vinyl alcohol)</t>
+          <t>PEDOT:PSS;</t>
         </is>
       </c>
     </row>
@@ -2052,7 +2055,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>PTCDA; TTF-TCNQ</t>
+          <t>tetrathiafulvalene-2,5-dichloro-p-benzoquinone;</t>
         </is>
       </c>
     </row>
@@ -2062,7 +2065,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>The OMIEC polymers mentioned in the text are; None.</t>
         </is>
       </c>
     </row>
@@ -2082,7 +2085,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>poly(gT2-T2), CNg4T2-CNT2</t>
+          <t>gT2; CNg4T2-CNT2</t>
         </is>
       </c>
     </row>
@@ -2092,7 +2095,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Naphthalenediimides; Arylenediimides; Viologens</t>
+          <t>Ionic arylenediimides; electron-rich ionic arylenediimides</t>
         </is>
       </c>
     </row>
@@ -2102,7 +2105,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>PEDOT:PSS</t>
+          <t>PEDOT:PSS;</t>
         </is>
       </c>
     </row>
@@ -2112,7 +2115,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Ppy-PSS; P3HT-Thionapthene; PTh-TTF; P3OT-CuPc; PPEvT-TTP</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2132,7 +2135,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Poly((9,9'-(4-(N-carboxy)phenylene)-bis-N,N-bis(2'-ethylhexyl)-3,6-bis(4-(2-ethylhexyl)-phenylene)thiourea)); PTCLI-Pt(II) complex</t>
+          <t>Polymer; PEI-PVMA-CuO; PEI-Bi-PVMA-CuO</t>
         </is>
       </c>
     </row>
@@ -2142,7 +2145,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Poly[N,N'-bis(2,2,2-trifluoroethyl)perylene-3,4-bis(carboxy-2-n-decyl-C5H14O4T); Poly{(9,9-dioctyl-2-fluorenyl-1,3-bis(2-carboxy-2-n-decylimino)propane}; Poly(3,4-ethylenedioxythiophene)-block-Poly(styrenesulfonate) (PEDOT:PSS);</t>
+          <t>Polymerized ionic liquid; Polyaniline-poly(styrenesulfonate); PSS-PVN; MEH-PVV; PEDOT-PSS.</t>
         </is>
       </c>
     </row>
@@ -2152,7 +2155,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>MA; MAPbI3; MAPbBr3; MAPbCl3; MAPb(ClBr)(3); MAPb(BrI)(3)</t>
+          <t>MA-based polymers;</t>
         </is>
       </c>
     </row>
@@ -2172,7 +2175,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>P4E4</t>
+          <t>P4E4:PEO</t>
         </is>
       </c>
     </row>
@@ -2182,7 +2185,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>IMI1,2O1TFSI; IMI1,1O2O1TFSI; BuMeIMITFSI</t>
+          <t>IMI1,2O1TFSI; IMI1,1O2O1TFSI</t>
         </is>
       </c>
     </row>
@@ -2192,7 +2195,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>P[(PNIPAM-PA)₂, P(NIPAM-PMAPT)₂, P(PAA-PMAPT)₂, P(PBA-PMAPT)₂, P(PSt-PMAPT)₂]</t>
+          <t>Polymeriophene; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-butylthiophene) (PBTT); Polyaniline; Poly(3-hexylthiophene) (P3HT); Poly(phenylenevinylene) (PPV); Poly(2-methoxy-5-(2'-ethyl-hexyloxy)-p-phenylenevinylene) (MEH-PPV)</t>
         </is>
       </c>
     </row>
@@ -2202,7 +2205,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT)/Poly(styrenesulfonate) (PSS)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2222,7 +2225,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>P(NDIEG7-FSVS); P(NDIOD-FSVS)</t>
+          <t>P(NDIEG7-FSVS); P(NDIOD-FSVS); Pg4NDI-T2; Pg4NDI-gT2; PNDI</t>
         </is>
       </c>
     </row>
@@ -2232,7 +2235,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>PSSHPT; PFOH-TPD; F16CuPc; Poly(3,4-ethylenedioxythiophene); PTDA-T; PTPA; PEDOT:PSS; Poly[2-methoxy-5-(2'-ethylhexyloxy)-1,4-phenylenevinylene]; Poly(9,9-dioctylfluorene)-b-poly(4,4'-bis(2-ethylhexoxy)-2,2'-bithiophene)</t>
+          <t>Conjugated Polymers-Poly(2,2'-Bithiophene)-5-Alkoxy-3,4-Cyclopentadithiophene; Poly(3,4-Ethylenedioxythiophene); Poly(3-Methylthiophene); Poly(3-Hexylthiophene); Poly(3-Octylthiophene); Poly(9,9-Dioctylfluorene); Poly(3-Butylthiophene); Poly(3-Dodecylthiophene); Poly(3-Tetradecylthiophene)</t>
         </is>
       </c>
     </row>
@@ -2242,7 +2245,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)-based; Poly(2,2',7,7'-tetrakis-(ethylene-3,4-(2-methoxy-5-methyl-phenyl))-spiro-bilindeno[2,1-a]isoindole))-based; Poly(3,3'-dioctyl-2,2'-bithiophene)-based; Poly(vinyl acetate)-based; Poly(styrene)-based</t>
+          <t>PEDOT:PSS; Polyaniline; Poly(3,4-ethylenedioxythiophene)-Poly(styrenesulfonate)</t>
         </is>
       </c>
     </row>
@@ -2252,7 +2255,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Poly[2,2'-azobipyridine-ru(bpy)(2)]; Poly(o-benzoquinonediimine-ru(bpy)(2))</t>
+          <t>bpz-abpy-bqdi;</t>
         </is>
       </c>
     </row>
@@ -2262,7 +2265,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>(BEDO-TTF)(Cl2TCNQ); (BEDT-TTF)(ClMeTCNQ)</t>
+          <t>(BEDO-TTF)(Cl(2)TCNQ); (BEDT-TTF)(ClMeTCNQ)</t>
         </is>
       </c>
     </row>
@@ -2272,7 +2275,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Poly(alkoxyphosphazene)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2282,7 +2285,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly vinylidene fluoride-trifluoroethylene (PVDF-TrFE); Poly (3-methylthiophene) (PMT); Poly (1,4-dioxan-2,3-diyl-alt-3,4-dimethyl-2,5-thienylene) (PDT-DM); Poly [2,7-(9,9-dioctylfluorene)-alt-4,7-bis(3,5-di-t-butylphenyl)-2,1,3-benzothiadiazole] (PFO-BT); Poly(phenyl-2,5-bis(3,5-dioctoxyphenyl)phenylene) (PPy-BDO); None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2292,7 +2295,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Polymer; Poly(3,4-ethylenedioxythiophene) (PEDOT)</t>
+          <t>Polyvinylcarbazole; Poly(methylphenylsilane); Polyaniline; Poly(3,4-ethylenedioxythiophene)</t>
         </is>
       </c>
     </row>
@@ -2322,7 +2325,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate) semi-crystalline regioregular polythiophene</t>
+          <t>oligoethylene glycol modified regioregular polythiophene</t>
         </is>
       </c>
     </row>
@@ -2342,7 +2345,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)-polystyrenesulfonate; Poly(3-octylthiophene)-PF6; Poly(3,4-ethylenedioxythiophene)-camphor sulfonate; None</t>
+          <t>Polymer; Poly(diacetylene); Poly(thienylenevinylene)</t>
         </is>
       </c>
     </row>
@@ -2372,7 +2375,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>P3HT/PSS; PEDOT:PSS; poly(3,4-ethylenedioxythiophene)-poly(4-styrenesulfonate); poly(3-hexylthiophene)-poly(styrenesulfonate)</t>
+          <t>Polymer; Poly(3,4-ethylenedioxythiophene)-based OMIEC polymer; Poly(3,4-ethylenedioxythiophene) (PEDOT)-based OMIEC polymer</t>
         </is>
       </c>
     </row>
@@ -2382,7 +2385,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>LiMoS2(PEO)(0.5); LiMoS2(PEO)(1.0)</t>
+          <t>Li1-xP3N(x)2O; Li0.1MoS2(PEO)(0.5); Li0.1MoS2(PEO)(1.0); PEO; LiPON</t>
         </is>
       </c>
     </row>
@@ -2392,7 +2395,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>PVP-PKHH; PPV-PPY; PEDOT-PSS; PANI-PSS; PMDA-PFSA; PVF-HFBT; P3HT-ET; Nafion-PEGDA</t>
+          <t>PANI-f-CFP;poly(Ethylene Oxide)-based OMIEC;PEDOT-PSS-co-PEO</t>
         </is>
       </c>
     </row>
@@ -2402,7 +2405,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>PEHT-GO; P3HT-EG; P3HT-EG-EL; P3HT-EG-PE</t>
+          <t>Polythiophenes</t>
         </is>
       </c>
     </row>
@@ -2412,7 +2415,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>beta-myrcene radical pendant polymer; radical polymer</t>
+          <t>Gamma-myrcene-based polymer; beta-myrcene-based polymer</t>
         </is>
       </c>
     </row>
@@ -2442,7 +2445,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>PolyEPz; PEDOT-SO3; PEDOT-PSS; P3HT-DBSA; Pd-Ppy; PPy-CaSO4; P3AT-DBSA</t>
+          <t>Polymer materials: P(VDF-TrFE); P(3HB-co-3HP); Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3,4-propylenedioxythiophene) (PProDOT).</t>
         </is>
       </c>
     </row>
@@ -2492,7 +2495,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Pentacene; Poly(3-hexylthiophene); Poly(3,4-ethylenedioxythiophene); Poly(phenylene vinylene); Polyfluorene; Poly(2-methoxy-5-(2-ethlyhexyloxy)-1,4-phenylene vinylene)</t>
+          <t>PEDOT:PSS; P3HT; Polyfluorene; MDMO-PPV; MEH-PPV</t>
         </is>
       </c>
     </row>
@@ -2502,7 +2505,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene); Poly(ethylene dioxythiophene) (PEDOT); Poly(dioxythiophene vinylene); Poly(2,2'-bithiophene); Poly(3-butylthiophene); Poly(3-octylthiophene)</t>
+          <t>Poly(3,4-ethylenedioxythiophene)(PEDOT); Poly(3,4-ethylenedioxythiophene) - poly(styrenesulfonate) (PEDOT-PSS); Poly(phenylthiophene-phenylvinylene) (PPTPV); Poly(ethylene oxide) (PEO); Poly(phenylthiophene-2,5-diyl) (PPT); Poly(3-thiopheneacetic acid) (PTAA); Poly(1-naphthyl-terminated) poly(ethylene oxide) (PnTEO); Poly(phenylthiophene-co-phenylvinylene) (PPTV); Poly(phenylselenophene-phenylvinylene) (PSPV)</t>
         </is>
       </c>
     </row>
@@ -2512,7 +2515,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Poly(ethylene-2,5-diimine); Poly(N-methyl-2,5-diiminopyridine); Poly(N-ethyl-2,5-diiminopyridine)</t>
+          <t>Polymer materials type OMIEC: None</t>
         </is>
       </c>
     </row>
@@ -2522,7 +2525,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>DPP-DODHT; DPP-DTP; P3HT-COOH; PSePh-TCNQ; PEDOT-COOH; PEO-PSS; PEO-PVB; PVK-COOH; PVP-PI; PVK-TCNQ</t>
+          <t>DPP-based copolymers</t>
         </is>
       </c>
     </row>
@@ -2542,7 +2545,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>TTF-DMDCNQI;</t>
+          <t>DMDCNQI-TTF;</t>
         </is>
       </c>
     </row>
@@ -2552,8 +2555,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>PEDOT-PSS; PSS-Fe; P3HT-Thiophene-FTAA; PANI-DBSA; PBTTT-C10-Thiophene-C14; PEF-PDOP; 
-(Note: Please keep in mind that the actual presence of these polymers in the original text cannot be guaranteed, but based on the information provided, these polymers can be inferred as OMIEC type.)</t>
+          <t>poly(3,4-ethylene dioxythiophene) (PEDOT); poly(3-hexylthiophene) (P3HT); Conjugated Polyelectrolyte; poly(2,5-bis(3-(benzo[d]thiazol-2-yl)-2-methylpropyl)-1,3,4-thiadiazole) (PBTTT); poly(2-methoxy-5-(2'-ethyl-hexyloxy)-p-phenylenevinylene) (MEH-PPV); poly(fluorene-alt-benzothiadiazole) (Poly(FBT)); poly(2-(3-thienyl)ethoxy-4,7-dithienylphenylene vinylene) (PThENVV);</t>
         </is>
       </c>
     </row>
@@ -2573,7 +2575,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>poly(3,4-ethylenedioxythiophene):polystyrene sulfonate</t>
+          <t>poly(3,4-ethylenedioxythiophene):polystyrene sulfonate (ZPS)</t>
         </is>
       </c>
     </row>
@@ -2583,7 +2585,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>PPO; PDIP; TTF-DMDOPOP; HPT; TTF-TCNQ</t>
+          <t>PMDT-TTF; PEDOT-PSS; DQNM-TTF; α-NPD; τ-X; β-NPD</t>
         </is>
       </c>
     </row>
@@ -2593,7 +2595,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>MoO3-pentacene; MEH-PPV: PFN; NPZ: PFN; F8T2: FAP; P3HT: [PBI]2HSO4</t>
+          <t>Pentacene;</t>
         </is>
       </c>
     </row>
@@ -2603,7 +2605,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Polymer-Naphthalenediimide-Thiophene; Poly(thiophene-alt-2,2'-(2-ethoxyethane)-5,5'-di(2-(triethylsilylethynyl)bisoindole)); None</t>
+          <t>Thiophene- triethylene glycol</t>
         </is>
       </c>
     </row>
@@ -2623,7 +2625,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; None</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -2633,7 +2635,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Li0.1MoS2(HNMe2)(y); Li0.1MoS2(HNEt2)(y)</t>
+          <t>Li0.1MoS2(HNR2)(y)</t>
         </is>
       </c>
     </row>
@@ -2643,7 +2645,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Tetrathiafulvalene-p-chloranil;</t>
+          <t>TTFC;</t>
         </is>
       </c>
     </row>
@@ -2653,7 +2655,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Poly(vinyl biphenylidene dicarboxylate); (TTF-CA)2; (TTF-DCA)2; TTF-TCNQ; F(TCNQ)2; (TTF-TCNQ)3; (TTF-F4TCNQ)2</t>
+          <t>Poly(p-phenylenevinylene-benzochalcogenophenone) (PBBPhene); Poly(2,2'-bithiophene-5-carboxylate) (1); Poly(3,3'-bithiophene-2,2'-(2,5-thiophenediyl)) (2); Trans-polyacetylene; Poly(2,5-bis(3-(phenyl)-2-thienyl)-3-thiophene) (1); Poly(3,4-bis(1,1-bis(m-trimethylsilylphenylmethan)-2-thienylmethoxy)thiophene) (1)</t>
         </is>
       </c>
     </row>
@@ -2663,7 +2665,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Polypyrrole; PEDOT; PTh; P3HT; poly-3,4-ethylene dioxythiophene; poly(2-methoxy aniline); poly(anthraquinonylthiophene)</t>
+          <t>P3HT:IC3MIM-PSI;PEI-PSSA-PSS;PEDOT:PSS;PMEH-PPV;PThiophene-PSS</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2675,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>P(NDI2OD-T2); poly(S)-b-poly(VBBI+[TFSI-]-r-PEGMA); poly(S)-b-poly(VBBI+[PF6-]-r-PEGMA); poly(S)-b-poly(VBBI+[BF4-]-r-PEGMA)</t>
+          <t>poly{[N,N'-bis(2-octyldodecyl)-naphthalene-1,4,5,8-bis(dicarboximide)-2,6-diyl]-alt-5,5'-(2,2'-bithiophene)}; poly(S)-b-poly(VBBI+[X]-r-PEGMA)</t>
         </is>
       </c>
     </row>
@@ -2683,7 +2685,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Polyvinylcarbazole; poly(2,5-bis(3-tetradecylthiophen-2-yl)thieno[3,2-b]thiophene); poly[2,2'-bithiophene]-5-carboxyaldehyde; poly(3,4-ethylenedioxythiophene)</t>
+          <t>EDOT-TTF; (PTT-TTF)2VO(NCS)2; ET-F2TCNQ; TTF-CA; F4TCNQ</t>
         </is>
       </c>
     </row>
@@ -2693,7 +2695,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Polymer(s): Poly(3,4-ethylenedioxythiophene)-based; Poly(3-hexylthiophene-2,5-diyl) unit;</t>
+          <t>Hf2CO2; Hf2COBr; Hf2COCl; Hf2COP; Hf2COOH; Hf2COS; Hf2COSe</t>
         </is>
       </c>
     </row>
@@ -2703,7 +2705,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)-nickel(II)bis(dithiolene); Poly(diketopyrrolopyrrole-thienothiophene); Poly(phenylenevinylene-benzophenone); PEDOT-PSS; Poly(3-hydroxythiophene); PEDOT-SnOx</t>
+          <t>Poly(p-phenylenevinylene-bitrifluoromethanesulfonate); Poly(3,4-ethylenedioxythiophene)-poly(4-styrenesulfonate); None</t>
         </is>
       </c>
     </row>
@@ -2713,7 +2715,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Poly-p-phenylene-vinylene-sulfonate/triarylamine; Poly(2-methoxy-5-(2'-ethylhexyloxy)-p-phenylene-vinylene); None</t>
+          <t>BzTMC(60); BzTiC(60)</t>
         </is>
       </c>
     </row>
@@ -2723,7 +2725,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Poly(di-n-octyl-3,4-ethylenedioxithiophene-alt-2,5-di-n-octyl-3,4-bis(generally acceptable alkyl thio)phenylene); (PTCDA-DTT); F4TCNQ-TTF; PEDOT-PSS; F6TCNQ-TTF; MEH-PPV-T1A; F16CuPc-IDTTF; PEDOT-PF6; F8TCNQ-TTF; N,N'-Bis(3- methyloxycarbonyl) phenyl-3,4,9,10-perylenediimide-TTF; PFCl6-12; None</t>
+          <t>N,N'-Diheptyl-3,4,9,10-perylenedicarboximide; Benzochrysene; TTF-DMTCN; PTCDI; DPTCDI-TCNQ; DPE-TCTDI; Diazetryptycene; PTCTP</t>
         </is>
       </c>
     </row>
@@ -2743,7 +2745,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Naphthalenediimide-based copolymer</t>
+          <t>naphthalenediimide-based copolymer</t>
         </is>
       </c>
     </row>
@@ -2753,7 +2755,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>P3HT-PAH; PEDOT-PSS; PPy; poly(3,4-ethylenedioxythiophene) (PEDOT); polyfluorene; poly(3-hexylthiophene) (P3HT); poly(ethylene oxide) (PEO); polypyrrole (PPy); poly(ethyl vinyl acetate) (EVAc); poly(vinylidene fluoride-co-hexafluoropropylene) (PVDF-HFP)</t>
+          <t>Polymer; gelatin-based solid-state electrolyte</t>
         </is>
       </c>
     </row>
@@ -2763,7 +2765,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>PPE-TT; PEDOT-TSF; PSS; PEOT; P3HT; PEDOT; PTh; PT; PFO; PVK; PANI-Thiacarbocyanine; P3AT; P3OT</t>
+          <t>PEDOT:PSS; PANI; P3HT; PPV; PEBV; PiNVI; PTh; PTh-CT; PNPB; PSI; Polyaniline-EDOT; Poly-thiophene-imide; PPy-PT; PPy-TrHB; PPV-PT; PBTT; P-NDI; P-NDI2OD-T; P-NDI3OD-T; P-NDI3OT-T</t>
         </is>
       </c>
     </row>
@@ -2773,7 +2775,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>PEDOT-PSS; PEDOT-Poly(4-vinylpyridine) carbonate; PEDOT-Poly(4-vinylpyridine) triflate</t>
+          <t>PEDOT-PSS; PEDOT-based materials</t>
         </is>
       </c>
     </row>
@@ -2783,7 +2785,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Polythiophene; naphthalene diimide-based polymer</t>
+          <t>polythiophene; naphthalene diimide-based polymer</t>
         </is>
       </c>
     </row>
@@ -2793,7 +2795,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>PSSDT; P3HT-TFSI; EDOT-TSF; PEDOT:PSS; PMeDOTT-TTF</t>
+          <t>PEDOT;PSS;PEDOT-PSS;PTh;PTAA;PTCDA;P3HT;P4VP;PMMA;Poly((9,9-diethylfluorene)-alt-(benzo[2,1,3]thiadiazole));Poly((9,9-diethylfluorene)-alt-(2-carboxy-2-cyclopropyl-ethenyl-benzaldehyde));Poly(2-methoxy-5-(2'-ethylhexyloxy)-1,4-phenylenevinylene);Poly(3-methylthiophene);Poly(3-thiophene acetic acid);Poly(3,4-ethylenedioxythiophene);Poly(3,4-ethylene dioxythiophene);Polythiophene;Polyaniline</t>
         </is>
       </c>
     </row>
@@ -2803,7 +2805,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>PBFDO;</t>
+          <t>PBFDO</t>
         </is>
       </c>
     </row>
@@ -2813,7 +2815,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>P3HT(AlHCF6)-PVOH; PANI-BTCA; PPy-DOT; PTh-DCTS; P3AT-DCA; PBTTT-C12; PDA-TFSI</t>
+          <t>Poly[(9,9-dioctyl-3-undecyl-2,7-carbazole)-(4,6-bis((7-octanoxythien-3-yl)oxy)-1,3-benzoxazole)])</t>
         </is>
       </c>
     </row>
@@ -2823,7 +2825,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>PTT2; Poly(1,4-phenylene-ethynylene); DCMU-PTEG</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2843,7 +2845,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>TTF-CN; Tetrathiafulvalene-chloranil</t>
+          <t>Tetrathiafulvalene-chloranil;</t>
         </is>
       </c>
     </row>
@@ -2853,7 +2855,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poly(3,4-ethylenedioxylthiophene)-based conjugated polymer; Prussian blue analogues; Poly(3-hexylthiophene) (P3HT); Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate) (PEDOT:PSS); Poly(3,3"-dihexyl-2,2'-bithiophene) (PDHT); Poly(ethylene oxide) (PEO); Poly(3-dodecylthiophene) (PDDT); Poly(3-octylthiophene); Poly(thieno[3,4-b]thiophene) (PTT); Poly(thieno[3,2-b]thiophene); </t>
+          <t>PDS-PbIxE; Polymeric Ferrocene-Tetracyanoquinodimethane Blends</t>
         </is>
       </c>
     </row>
@@ -2903,7 +2905,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Polymer electrolyte 6,5-dimethyl-2,2'-bithiophene-alt-5,5'-bis(4-biphenylyl)-2,2'-bithiophene; MEH-PPV; PEDOT-PSS/TiO2; P3HT; PCEBT; PBTTT-C8; F8BT; PFO; PFVT; PBT; PBTTT; P3OT; PBTT; PFOCT; P4PV; P3PV; PBTTT-C10</t>
+          <t>Poly-(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); Perylene-diimide-based polymers</t>
         </is>
       </c>
     </row>
@@ -2913,7 +2915,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>PPEAH; PVC; PEDOT-PSS; Poly(3,4-ethylenedioxythiophene) - Poly(styrenesulfonate); PTB; Poly(thiophene-3-acetic acid)</t>
+          <t>Parylene-Octadecylphosphonic acid; Poly(ethylene oxide)-block-poly(butylene oxide); Poly(3,4-ethylenedioxythiophene) (PEDOT)</t>
         </is>
       </c>
     </row>
@@ -2923,7 +2925,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>PET-TTF; TTF-CA; TTF-CCNQ</t>
+          <t>tetrathiafulvalene-p-chloranil</t>
         </is>
       </c>
     </row>
@@ -2953,7 +2955,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>PEDOT;</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -2963,7 +2965,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PEDOT:PSS; P3HT; PEO; PIBF-5; PTh; PVK-FTAA; PCT; PEM; PBTT; PBTTT; PFO-Th; PFO-Th; P3HT-Th; MeO-3CzT-PDPP-TT; CPZF; PNP; NDCs-TTF; (PhPyDTTS)2-C4F8; (PhPyDTTS)2-C4F6</t>
+          <t>PEDOT:PSS; Polymers derived from imidazolium-type ionic liquids; Polymers derived from thiol-terminated imidazolium-type ionic liquids</t>
         </is>
       </c>
     </row>
@@ -2973,7 +2975,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Poly(3-hydroxythiophene); P3HT-PCBM; P(CDC)P; PTB7-Th; PDPP-3T-T; P(NDI2OD-T2)</t>
+          <t>Methylammonium lead iodide (CH3NH3PbI3)</t>
         </is>
       </c>
     </row>
@@ -2983,7 +2985,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; PANI; Ppy; Poly(3,4-ethylenedioxythiophene); PTh;</t>
+          <t>Poly(vinylphenol-co-3,4-ethylenedioxythiophene); PEDOT:PSS; Poly(3,4-ethylenedioxythiophene); Polypyrrole; Poly(aniline-co-o-aminophenol)</t>
         </is>
       </c>
     </row>
@@ -2993,7 +2995,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>PMDT-TBA; BSPB; TTF-TCNQ; DMe-bis-TTF; TCNQ-TCNQ; BETS; TTF-CuPz; Me4TTF; TTF-CuTBP; MEH-PPV; F4TCNQ-TCNQ; BIS(TTF)Cu; EDOT-TTP-TTF; BMH-Phen; TTF-CuBr-Phen; F4TCNQ-TCNQ-F4TCNQ; TED; TTF-CuBr-DMF; EDOT-TTP-DOT; BIS(TTF)Cu-TTF; TTF-DCA; TTF-CuTBP-TTF; F4TCNQ-Phen-F4TCNQ; BMH-Phen-BMH; TTF-CuPz-TTF; TTF-TET; TTF-CuBr-DMF-TTF; EDOT-TTP-DOT-DOT;</t>
+          <t>polyN-Vinylcarbazole; polyfluorene; polythiophene; poly(phenylene-vinylene); poly(phenylene-sulfide); poly(phenylene-ethylene)</t>
         </is>
       </c>
     </row>
@@ -3003,7 +3005,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>bis(3,4-ethylenedichalcogenothiophene)-fluorinated tetracyanoquinodimethanes;</t>
+          <t>Bis(3,4-ethylenedichalcogenothiophene)-fluorinated tetracyanoquinodimethanes;</t>
         </is>
       </c>
     </row>
@@ -3073,7 +3075,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>DHBQDS-Na-carbon nanocomposite</t>
+          <t>DHBQDS</t>
         </is>
       </c>
     </row>
@@ -3083,7 +3085,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Potassium terephthalate;</t>
         </is>
       </c>
     </row>
@@ -3093,7 +3095,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>TTF-CA;</t>
+          <t>TTF-CA</t>
         </is>
       </c>
     </row>
@@ -3103,7 +3105,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>HKUST-1;UiO-66</t>
         </is>
       </c>
     </row>
@@ -3113,7 +3115,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Poly[2-methoxy-5-(2-ethylhexyloxy)-1,4-phenylenevinylene- alt-1,4-benzoquinone]; Poly[5-(2-ethylhexyloxy)-1,4-phenylenevinylene- alt-1,4-benzoquinone]; Poly[N,N'-bis(2,2,2-trifluoro-1-methylethyl)-3,5-diamino-4-hydroxy-benzoic acid];</t>
+          <t>PyPIL</t>
         </is>
       </c>
     </row>
@@ -3123,7 +3125,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Poly[3,4-ethylenedioxythiophene-poly(styrenesulfonate)]; Poly(3-methyliodostyrene); Poly(3,4-ethylenedioxythiophene-co-3-methyliodostyrene); None</t>
+          <t>PBEDTTF;Poly(3-methyl-thiophene);Poly(3-hexylthiophene);Poly(3-decyltetradecylthiophene);Poly(3-alkylthiophene)</t>
         </is>
       </c>
     </row>
@@ -3143,7 +3145,8 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Poly(ethylenedioxythiophene) (PEDOT); Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate) (PEDOT-PSS); Poly(3,4-ethylenedioxythiophene)-poly(4-styrenesulfonate) (PEDOT-PSS); Poly(3,4-(2',3'-dihexylthieno-[3,4-b]-thienylene-ethynylenedioxythiophene) (6EGT-PEDOT); Poly(3,4-ethylenedioxythiophene) - poly(styrenesulfonate) doped with Poly(ethylene oxide) (PEDOT-PSS-PEO); Poly(3,4-ethylenedioxythiophene) - poly(styrenesulfonate) doped with Poly(vinyl acetate) (PEDOT-PSS-PVA); Poly(3,4-ethylenedioxythiophene) - poly(styrenesulfonate) doped with Poly(vinyl alcohol) (PEDOT-PSS-PVA); Poly(3,4-ethylenedioxythiophene) - poly(styrenesulfonate) doped with Poly(acrylic acid) (PEDOT-PSS-PAA)</t>
+          <t>PEDOT:PSS; P3HT:ICl; PPV-CuPc; 
+(Note: OMIEC polymers mentioned in the text)</t>
         </is>
       </c>
     </row>
@@ -3153,7 +3156,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>PEDOT-PSS; Poly(3,4-ethylenedioxthiophene)-poly(styrenesulfonate); Polytfluorene-vinylbenzyl sulfonate; Poly(2-methoxy, 5-(2''-ethyl-hexyloxy)-1,4-phenylenevinylene)-polystyrenesulfonate; Poly[2,5-di(2-benzo-thiazolyl)-p-phenylene-ethynylene]-polystyrenesulfonate; Poly[2-methoxy, 5-(2''-ethyl-hexyloxy)-1,4-phenylenevinylene]-poly(toluenesulfonate)</t>
+          <t>Polymeric Naphthalene Diimide (PNDI); Poly(3,4-ethylenedioxthiophene) (PEDOT); Polyfluorene; PSSH-PTT; PTh-PEI; Conjugated Polyfluorene; PTh-PEG; PEDOT:PSS; PTh-PTMC; Polythiophene; PEDOT-SO3</t>
         </is>
       </c>
     </row>
@@ -3173,7 +3176,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Poly(THBP)</t>
+          <t>Poly(alkyl naphthalene) imidazolium dicyanamide</t>
         </is>
       </c>
     </row>
@@ -3183,7 +3186,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>PEDOT:PSS;</t>
+          <t>Poly(3,4-ethylenedioxythiophene) polystyrene sulfonate (PEDOT:PSS)</t>
         </is>
       </c>
     </row>
@@ -3193,7 +3196,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Polymer ionic metal (PIM); PEDOT-PSS; PANI; PPy; PTh; PTh-MeOH; PEDOT; PVP; PEO; PAN; PBPP; P3HT; PBTTT</t>
+          <t>PolymerFET; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(thiophene); PEDOT:PSS; Poly(3-hydroxybutyrate) (PHB); Poly(vinylidene fluoride-co-trifluoroethylene) (P(VDF-TrFE)); PEDOT-grafted-poly(ethylene oxide) (PEDOT-g-PEO); Poly(aniline) (PAni); PEDOT-cysteamine (PEDOT-CS); Poly(sulfidylenemethylene-co-vinylene) (PSM-co-V); PEDOT-butansulfonic acid (PEDOT-BSA); PEDOT-imidazole (PEDOT-imid); Poly(styrenesulfonate) (PSS); PEDOT-γ-cyclodextrin (PEDOT-γ-CD); PSulfonated polyaniline (SPAni)</t>
         </is>
       </c>
     </row>
@@ -3203,7 +3206,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Polymer;Poly[2-methoxy-5-(2'-ethyhexyloxy)-1,4-phenylenevinylene)-COOPicolinate]</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3213,7 +3216,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Polyvinylcarbazole; Poly(3,4-ethylenedioxythiophene); Polypyrrole; Poly(aniline); Poly(3-hexylthiophene)</t>
+          <t>Poly(3,4-ethylenedioxythiophene)-based OMIEC; Poly(diketopyrrolopyrrole)-based OMIEC</t>
         </is>
       </c>
     </row>
@@ -3223,7 +3226,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>LiNi0.5Mn0.3Co0.2O2; LiMn1.5Ni0.5O4</t>
         </is>
       </c>
     </row>
@@ -3233,7 +3236,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>1-Ethyl-3-methylimidazolium acetate; 1-ethyl-3-methylimidazolium chloride; 1-ethyl-3-methylimidazolium thiocyanate; 1-ethyl-3-methylimidazolium trifluoroacetate; 1-ethyl-3-methylimidazolium tetrafluoroborate; 1-ethyl-3-methylimidazolium methanesulfonate; 1-ethyl-3-methylimidazolium bis(trifluoromethanesulfonyl) imide</t>
+          <t>1-ethyl-3-methylimidazolium acetate; 1-ethyl-3-methylimidazolium chloride; 1-ethyl-3-methylimidazolium thiocyanate; 1-ethyl-3-methylimidazolium trifluoroacetate; 1-ethyl-3-methylimidazolium tetrafluoroborate; 1-ethyl-3-methylimidazolium methanesulfonate; 1-ethyl-3-methylimidazolium bis(trifluoromethanesulfonyl)imide</t>
         </is>
       </c>
     </row>
@@ -3253,7 +3256,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>(3-(dibenzo[c,h]acridin-7-yl)phenyl)di-phenylphosphine oxide-lithium-8-hydroxyquinolinolate;</t>
+          <t>(3-(dibenzo[c,h]acridin-7-yl)phenyl)di-phenylphosphine oxide; 8-hydroxyquinolinolato-lithium</t>
         </is>
       </c>
     </row>
@@ -3263,7 +3266,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>FelixAPC; PCE8; Poly(3-hexylthiophene)-based OMIEC; PTAA; PBTTT; F16CuPc; P3HT-E; P(NDI2OD-T2); PBTT-T; PBTT-E; PCE6; P(NDI2OD-T2); TPAHB; PBTT2-T; PMDT-T; PMDA9T10.</t>
+          <t>Guanidinium ion-based organic-inorganic halide perovskite</t>
         </is>
       </c>
     </row>
@@ -3273,7 +3276,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Polymer names: Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(styrenesulfonate) (PSS); Poly(phenylenevinylene) (PPV); Poly(3-hexylthiophene) (P3HT); Poly(3-butylthiophene) (P3BT); Poly(2-methoxy-5-(2-ethylhexyloxy)-p-phenylenevinylene) (MEH-PPV); Poly(indenofluorenone) (PIDFN); Poly(9,9-dioctylfluorene-alt-benzothiadiazole) (F8BT); Poly(2-methoxy-5-(2-ethylhexyloxy)-1,4-phenylenevinylene) (MEH-PPV); Poly(3,3-dioctyl-2,2'-bithiophene) (DDT-TT); Poly(thienothiophene) (PTT); Poly(1,4-bis(3,7-dimethyloctadecanoyl)stilbene-4,4'-diyl) (BZ); Poly(thiophene-alt-benzothiadiazole) (PT-BT); Poly(2,7-dioctyl-[1]benzothieno[3,2-b][1]benzothiophene) (BTBT); Poly(3,6-carbazole) (P3CB); Poly(2,7-dibromo-9,9-di-octylfluorene-alt-2,2'-(ethylene-1,2-di-yl)bis(4,4,5,5-tetramethyl-1,3,2-dioxaborolan)) (F8BT); Poly(9,9-dioctyl-3,6-bis-thiophen-2-yl-fluorene-2,7-diyl) (PFTT); Poly(3,6-dibromothieno[3,2-b]thiophene) (PBT); Poly(2,5-bis(3-ethyl-2-benzothiazolyl)thieno[3,2-b]thiophene) (PBT-EBT); Poly(3,4-phenylenevinylene) (PPV); Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(styrenesulfonate) (PSS); Poly(tetracyanoquinodimethane) (TCNQ); Poly(1,2-dimethoxy-4,5-bis(2,3-dihydroxy-5-propoxyphenyl)-benzene) (PDC);</t>
+          <t>PSS-TPD; PEDOT:PSS; Naphthalenediimide; Isoindigo; Fluoranthene-derivatives; π-conjugated polymers</t>
         </is>
       </c>
     </row>
@@ -3293,7 +3296,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Poly(2,2'-bithiophene-phenylene); Poly(phenylene-1,4-dithienylphenylene)</t>
+          <t>2,2'-bithiophene; 1,4-dithienylphenylene; phenylene</t>
         </is>
       </c>
     </row>
@@ -3313,7 +3316,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Poly(3-hexylthiophene-2,5-diyl); Poly-(trifluoromethanesulfonylimide)</t>
+          <t>poly(3-hexylthiophene-2,5-diyl); poly(trifluoromethanesulfonylimide)</t>
         </is>
       </c>
     </row>
@@ -3323,7 +3326,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)-polystyrene sulfonate; P3HT-PCBM; PEMA-MOF; PEPA-MOF; PEMeT-TET</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3333,7 +3336,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>P3HT-PMMA; PPy-CN; PEDOT:PSS; PTh-EBI; PVP-TFA; PI-PDDA; PEO-KBr; PMS-IPy; PMMA-EG; PVP-T; PAH-BA.</t>
+          <t>Polymer;</t>
         </is>
       </c>
     </row>
@@ -3343,7 +3346,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>(OM)(2)MImPF(6)</t>
+          <t>(OM)(2)MImPF(6); EDImPF(6); EMImPF(6)</t>
         </is>
       </c>
     </row>
@@ -3353,7 +3356,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; PANI:PSS; DPEPP; PT-DBS; Poly(3,4-ethylenedioxythiophene)-PEBB; PEIEB; Poly(3,4-ethylenedioxythiophene):Poly(styrene sulfonate); PEDOT-PPO; Poly(3-hexylthiophene)-CAM; PEDOT-PAA; PPy/PSS; PEDOT:PEOB; PVK:MAA; PEDOT-PFN; Pyrrole/ Poly(styrene sulfonate); PFS/PSS; PPy/PFSA.</t>
+          <t>PEDOT/PSS; PPy; PANI; PBTTT-C8; PTAA; P3HT</t>
         </is>
       </c>
     </row>
@@ -3363,7 +3366,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Polyvinylpyrrolidone; Poly(3,4-ethylenedioxythiophene)-Poly(styrenesulfonate); Poly(p-phenylene vinylene)</t>
+          <t>Polymer materials found: Ploemerein;</t>
         </is>
       </c>
     </row>
@@ -3373,7 +3376,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Polymer complexes of polyfluorene-triarylphosphine oxide; Poly(3,4-ethylene-dioxythiophene); Poly(phenylene vinylene); Pizzo; Poly(triphenylamine); Polyfluorene; Poly(phenylsulfone); Polybenzimidazole; PEDOT-TfS; PEDOT-PSS</t>
+          <t>P3HT; PEDOT:PSS; PANI; PPy; PEI; PSU</t>
         </is>
       </c>
     </row>
@@ -3383,7 +3386,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>PQPC(6)ClO4; PQPC(6)AQS; PQPC(6)BS</t>
+          <t>PQPC(6)(+) perchorate; PQPC(6)(+) anthraquinonedisulfonate; PQPC(6)(+) benzenesulfonate</t>
         </is>
       </c>
     </row>
@@ -3403,7 +3406,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>P-3O</t>
+          <t>P-3O;</t>
         </is>
       </c>
     </row>
@@ -3413,7 +3416,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Poly(3-(triethylene glycol)thiophene);</t>
+          <t>Triethylene glycol polymer;</t>
         </is>
       </c>
     </row>
@@ -3423,7 +3426,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>CPETBTT; P3HT-TFSI; PSSA-P3HT; PEDOT-PSS; PCBM-TFSI</t>
+          <t>CPEs</t>
         </is>
       </c>
     </row>
@@ -3443,7 +3446,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>P3HT/SEBS</t>
+          <t>P3HT; SEBS</t>
         </is>
       </c>
     </row>
@@ -3453,7 +3456,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>PMDT-TTNF; poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate) (PEDOT:PSS); PEDOT/PSS; PSS/PEO; PEDOT:PSS/PEG; PEDOT-graft-PSS; Poly(diallyldimethylammonium chloride); None</t>
+          <t>Polymer names: P3HT; PPE-DMT; PDIC-DMT; PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -3463,7 +3466,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>PMDA-PDA; PTAA-PF6; PSS-AuNP; PANI-EtSO3Ag; P3HT-Cu; PTAA-DEDA</t>
+          <t>h-WO3;</t>
         </is>
       </c>
     </row>
@@ -3483,7 +3486,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene); Poly(3-hexylthiophene); Poly(3-octylthiophene); Poly(9,9-dioctylfluorene); Poly(3,4-ethylenedioxy-2,5-thiophene); Poly(aniline-co-o-phenylenediamine); Poly(5,5'-dithiobis(2,2'-bithiophene))</t>
+          <t>Poly(ethylene dioxythiophene) (PEDOT); Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3,4-ethylenedioxylthiophene); Ppy; Poly(3-methylthiophene); Poly(aniline-co-o-anisidine)</t>
         </is>
       </c>
     </row>
@@ -3503,7 +3506,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>PDDTT-TTP; P3AT; P3HT; PCDTBT; None</t>
+          <t>NDI-T2-based n-type OECT material</t>
         </is>
       </c>
     </row>
@@ -3513,7 +3516,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Poly(pyrrole-bis(phenylene vinylene)); Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-hexylthiophene)/[BMIM][FeCl4]Ionic Liquid Blended; Poly(hexylthiophene); Poly(fluorene-co-benzothiophene)</t>
+          <t>Polymer;PEDOTS;P3HT;PBHT;PESA;PTECH</t>
         </is>
       </c>
     </row>
@@ -3523,7 +3526,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>PEDOT-PSS; PTh; Ppy; POFPT</t>
+          <t>Poly(3,4-ethylenedioxythiophene)Co(4-ethylphenolate); Poly(3,4-ethylenedioxythiophene)Co(4-butylphenolate); Poly(3,4-ethylenedioxythiophene)Co(4-hexylphenolate); Poly(3,4-ethylenedioxythiophene)Co(4-octylphenolate); Poly(3,4-ethylenedioxythiophene)Co(4-dodecylphenolate); Poly(3,3/-thiophene)Co(4-ethylphenolate); Poly(3,3/-thiophene)Co(4-butylphenolate); Poly(3,3/-thiophene)Co(4-hexylphenolate); Poly(3,3/-thiophene)Co(4-octylphenolate); Poly(3,3/-thiophene)Co(4-dodecylphenolate)</t>
         </is>
       </c>
     </row>
@@ -3533,7 +3536,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Perfluorobenzylammonium iodide; (perfluoro-1,4-phenylene)dimethylammonium iodide</t>
+          <t>Perfluoro-1,4-phenylene)dimethylammonium iodide; (perfluorobenzyl)ammonium</t>
         </is>
       </c>
     </row>
@@ -3553,7 +3556,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>p(ETE-S);</t>
+          <t>p(ETE-S)</t>
         </is>
       </c>
     </row>
@@ -3563,7 +3566,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>PEDOT:PSS;</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -3573,7 +3576,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Poly(-secondary-butylamine)-MoS2; Poly(secondary-hexylammine)-MoS2</t>
+          <t>SMAc; MIMS; P3MT</t>
         </is>
       </c>
     </row>
@@ -3583,7 +3586,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>PEDOT-PBA;</t>
+          <t>PEDOT-PBA</t>
         </is>
       </c>
     </row>
@@ -3603,7 +3606,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Poly[3,4-ethylenedioxythiophene]-poly(ethylene oxides); Poly(3,4-pyridinedione)-poly(ethylenedioxythiophene); Poly(3-methylthiophene)-poly(ethylene oxide)</t>
+          <t>Polymer; Poly(3,4-ethylenedioxythiophene); Poly(thiophene); Poly(aniline); Poly(3,4-ethylenedioxy-2,5-thiophene); Poly(o-phenylenediamine)</t>
         </is>
       </c>
     </row>
@@ -3613,7 +3616,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>P3HT/PEDOT:PSS; PEDOT:PSS/PVK; PEDOT:PSS/PAA; PMMA/PEDOT; PTh/PTAA; PTh/PTAA/PTh; PTh/PTAA/PTA; PTh/PTAA/PDEA; PTh/PTAA/PMAA</t>
+          <t>OCTIO; PEDOT:PSS; Poly(3,4-ethylenedioxythiophene); Poly(aniline-co-oanisidine); Poly(ethylenedioxythiophene)-poly(styrenesulfonate); PBTTT-Se; Nafion</t>
         </is>
       </c>
     </row>
@@ -3643,7 +3646,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Poly(thiophene-3-carboxybutyl); Poly(thiophene-3-carboxyethyl)</t>
+          <t>Polythiophene;</t>
         </is>
       </c>
     </row>
@@ -3653,7 +3656,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>PEDOT:PSS</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3673,7 +3676,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Pentacene; Tetrathiafulvalene; Poly(3,4-ethylenedioxythiophene)</t>
+          <t>P3HT : PTAA;</t>
         </is>
       </c>
     </row>
@@ -3693,7 +3696,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene); Poly(3-hexylthiophene); Poly(2-methoxy-5-(2-ethylhexyloxy)-1,4-phenylene vinylene); None</t>
+          <t>Spiro-MeOTAD</t>
         </is>
       </c>
     </row>
@@ -3703,7 +3706,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Poly[(9,9-dioctylfluoren-2-yl)thiophene-2-ylmethoxyborane]; Poly[9,9-dimethylfluoren-2-ylmethoxyborane]; Poly{[N,N'-bis(2,2'-bipyridin-6-yl)-{N,N'-bis(2,2'-bipyridin-6-yl)-{N,N'-bis(2,2'-bipyridin-                    </t>
+          <t>Poly(3-hexylthiophene); Poly(3,4-ethylenedioxythiophene)</t>
         </is>
       </c>
     </row>
@@ -3713,7 +3716,7 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxthiophene)-poly(ethylene oxide); Poly(4-vinylpyridine)-polystyrene; PVP-co-PSS</t>
+          <t>Poly[1-(3-methacryloyloxy-2-hydroxypropyl)imide-co-1-(3-methacryloyloxy-2-hydroxypropyl)sulfonate]; Poly(urethane-maleimide); None</t>
         </is>
       </c>
     </row>
@@ -3763,7 +3766,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>Naphthodithiophene diimide polymer;</t>
+          <t>NDTI-based polymer; naphthalene diimide (NDI) unit</t>
         </is>
       </c>
     </row>
@@ -3843,7 +3846,7 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>PEDOT:PSS</t>
+          <t>PEDOT:PSS;</t>
         </is>
       </c>
     </row>
@@ -3853,7 +3856,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>poly([Benzidine-iodine]])</t>
+          <t>Benzidine-Iodine complex; o-tolidine-Iodine complex</t>
         </is>
       </c>
     </row>
@@ -3863,7 +3866,7 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>P3HT-PVBA; PPy-PSSA; PEDOT-PSS; PEDOT-SiO2; PTh-SiW; VOPC; poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); PSSH; poly(3-dodecylthiophene)-poly(styrenesulfonate)</t>
+          <t>Polymerics; Poly[3,4-ethylenedioxythiophene]-poly(styrenesulfonate); none</t>
         </is>
       </c>
     </row>
@@ -3873,7 +3876,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>PEDOT:PSS</t>
+          <t>PEDOT:PSS; TEMPO+X-; TEMPO+TFSI-</t>
         </is>
       </c>
     </row>
@@ -3893,7 +3896,7 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>poly(3,4-ethylenedioxythiophene)-poly(4-styrenesulfonate); poly(3,4-ethylenedioxythiophene)- poly(styrenesulfonate); Poly(3-hexylthiophene)-Poly(styrenesulfonate); None</t>
+          <t>Poly(3-hexylthiophene)-[N,N'-di(2-(3-ethoxysilyl)ethoxy)-3,4,9,10-perylenedicarboximide] (P3HT-PECN); Poly(3-(2-(3-ethoxysilyl)ethoxy)thiophene)-[N,N'-di(3-ethoxysilyl)ethoxy)-3,4,9,10-perylenedicarboximide] (P3ET-PECN); Poly(3-ethoxysilyl)ethoxythiophene-[N,N'-di(2-(3-ethoxysilyl)ethoxy)-3,4,9,10-perylenedicarboximide] (P3ST-PECN); Poly(3-methylthiophene)-[N,N'-di(2-(3-ethoxysilyl)ethoxy)-3,4,9,10-perylenedicarboximide] (P3MT-PECN); Poly(3-butylthiophene)-[N,N'-di(2-(3-ethoxysilyl)ethoxy)-3,4,9,10-perylenedicarboximide] (P3BT-PECN)</t>
         </is>
       </c>
     </row>
@@ -3923,7 +3926,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>PMDHF, PMeDHF, PTCDI-based, BPE, BPE-based, MDMO-PPV, PANI-based, Nafion, P3HT, PEDOT, PEO-based, PFM, PMMA-based, PPy-based</t>
+          <t>PEEOTP; PEMeTT; PIPSA; PIFA; PETT; PAPP</t>
         </is>
       </c>
     </row>
@@ -3933,7 +3936,7 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>Polymerthane; Poly(N-vinylcarbazole); Poly(3-methylthiophene)-poly(vinylcarbazole); Poly(2-methoxy-5-(2'-ethylhexyloxy)-1,4-phenylenevinylene); None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3943,7 +3946,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>F6TCNNQ;</t>
+          <t>F6TCNNQ</t>
         </is>
       </c>
     </row>
@@ -3953,7 +3956,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>Polymer; none</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3963,7 +3966,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>Poly[3-methylthiophene]; Poly(fluorene); Poly(3-hexylthiophene); Poly(9,9-dioctylfluorene); Poly(diketopyrrolopyrrole-benzothiadiazole)</t>
+          <t>Poly(3-hydroxybutyrate); Poly(3-hydroxybutyric acid-co-3-hydroxyvaleric acid)</t>
         </is>
       </c>
     </row>
@@ -3983,7 +3986,7 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3,4-ethylenedioxythiophene)-poly(4-styrenesulfonate) (PEDOT-PSS); Poly(aniline-co-isoquinoline)</t>
+          <t>Poly[2-methoxy-5-(2-ethylhexyloxy)-1,4-phenylene vinylene]; Poly(3,4-ethylenedioxythiophene); None</t>
         </is>
       </c>
     </row>
@@ -4003,7 +4006,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>Polyvinylpyrrolidone; Poly(3, 4-ethylenedioxythiophene) (PEDOT); Polyaniline; Poly[2-methoxy-5-(2'-ethyl-hexyloxy)-1,4-phenylene vinylene] (MEH-PPV); Poly(phenylene vinylene) (PPV); Poly(epichlorohydrin-co-butyl vinyl ether) (PECBVE); Poly[3-(6-ferrocenylhexyl)thiophene]; None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4013,7 +4016,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>Poly(3-hydroxythiophene); Poly(3-methylthiophene); Poly(3-chlorothiophene); None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4033,7 +4036,7 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Ppy-CA</t>
         </is>
       </c>
     </row>
@@ -4053,7 +4056,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>Nafion/(ZrHf)(x); Nafion/(SiHf)(x)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4073,7 +4076,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>Polymer samples with OMIEC properties: MAPbI; GA; EPA; AcM</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4083,7 +4086,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>iCONs</t>
         </is>
       </c>
     </row>
@@ -4093,7 +4096,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>CPDT-g-PBTTT; CPDT-g-P3HT; CPDT-g-PDTT</t>
+          <t>CPDT-Gly1; CPDT-Gly2; CPDT-Gly3</t>
         </is>
       </c>
     </row>
@@ -4103,7 +4106,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>Polyvinyl Ferrocyanide; Poly(3,4-ethylene-2,5-dioxythiophene)-Poly(styrenesulfonate); Poly(3-hexylthiophene); None</t>
+          <t>P3HT:PSS; PEDOT:PSS; PTAA; PPy-DBSA; PTh-DBSA</t>
         </is>
       </c>
     </row>
@@ -4123,7 +4126,7 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; PANI; P3HT; PMMA; PPy; PBTTT-TTBT; PPC; PFO; Fluorinated polyimide; Poly(3,4-ethylenedioxythiophene); Poly(9,9-dioctylfluorene); Poly(thiophene-2-carboxylate); None</t>
+          <t>PEDOT:PSS;ppy-TTF;P3HT:ICBA;PSE;PDVN;PVS;P4VP;PVP;PANI</t>
         </is>
       </c>
     </row>
@@ -4133,7 +4136,7 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>OPBI</t>
+          <t>OPBI;</t>
         </is>
       </c>
     </row>
@@ -4143,7 +4146,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>Poly(2,3,6,7,10,11-hexahydroxytriphenylene) Co(II); Poly(2,3,6,7,10,11-hexaiminotriphenylene) Co(II); Poly(2,3,6,7,10,11-hexaiminotriphenylene) Cu(II); Poly(2,3,6,7,10,11-hexaiminotriphenylene) Ni(II)</t>
+          <t>HHTP-Polymer; HITP-Polyer</t>
         </is>
       </c>
     </row>
@@ -4163,7 +4166,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>Polymeroids; PEDOT-PSS; P3HT; PTh; PDOT; P3OT</t>
+          <t>Poly(3,4-ethylenedioxythiophene); Poly(p-phenylenevinylene); Poly(3-methylthiophene); Poly(thieno[3,2-b]thiophene); Poly(3,4-bis(thienyl)-thiophene);</t>
         </is>
       </c>
     </row>
@@ -4183,7 +4186,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1-Mo-8; 2-Mo-8; 1-PW12; 2-PW12</t>
         </is>
       </c>
     </row>
@@ -4193,7 +4196,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>Pyrrole-MethylRed-Polyaniline; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-hexylthiophene) (P3HT); Poly(3-methylthiophene) (P3MT);</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4253,7 +4256,7 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; PTAA; PTh; PPy; PTFE; PVK; TPB</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4263,7 +4266,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>Polyvinylcarbazole (PVCz); Poly(3,4-ethylenedioxythiophene)-block-Poly(styrene-sodium 4-styrenesulfonate) (PEDOT-PSS); Polypyrrole (Ppy); Polyaniline (PANI); Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3,4-ethylenedioxythiophene)-poly(ethylene oxide) (PEDOT-PEO); Poly(ethylene oxide)-block-Poly(ethylene glycol) (PEO-PEG); Polysulfone (PSF); Poly(vinylidene fluoride-co-hexafluoropropylene) (PVDF-HFP); Poly(3-methylthiophene) (PMeT); Polysiloxane; Poly(ethylene glycol) (PEG); Poly(vinylpyrrolidone) (PVP); Polyethyleneimine (PEI); Poly(vinyl acetate) (PVAc); Poly(4-vinyl pyridine) (P4VP); Poly(acrylic acid) (PAA); Poly(methyl methacrylate) (PMMA); Poly(2-methoxyethyl acrylate) (PMEA); Polyanthracene (PAn); Polyphenyl ether (PPE); Poly(2-vinyl pyridine) (P2VP)</t>
+          <t>Please input the text you want me to analyze.</t>
         </is>
       </c>
     </row>
@@ -4273,7 +4276,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>[CpTiCpCo](infinity); [CpTiCpFe](infinity); [CpCrCpCo](infinity); [CpCrCpFe](infinity); [CpFeCpCo](infinity)</t>
+          <t>[CpTiCpCo](infinity); [CpCrCpCo](infinity); [CpTiCpFe](infinity); [CpCrCpFe](infinity); [CpFeCpCo](infinity)</t>
         </is>
       </c>
     </row>
@@ -4303,7 +4306,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>PMDA-Co-PVP; P(St-Co-MMA); PEO-TIPS; PEM; PEO-NaPF6; PEI-PVDFHFP</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4313,8 +4316,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>Here are the OMIEC polymers mentioned in the text, separated by semicolons:
-None</t>
+          <t>2-ethynyl-1,3-dimethyl-1H-imidazol-3-ium hexafluorophosphate (1.PF6); 6-phenyl-4-(3,4,5-tris(dodecyloxy)phenyl)-2,2'-bipyridine)</t>
         </is>
       </c>
     </row>
@@ -4334,7 +4336,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>PTCPB; PTPMB; PTPE; PTPO; PTTPB</t>
+          <t>Poly(3-hydroxyquinuclidinium perchlorate); None</t>
         </is>
       </c>
     </row>
@@ -4354,7 +4356,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>(BEDT-TTF)(ClMeTCNQ); (TTF)(CA)</t>
+          <t>(BEDT-TTF)(ClMeTCNQ)</t>
         </is>
       </c>
     </row>
@@ -4374,7 +4376,7 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>Poly(thiophene-co-ethylene glycol);</t>
+          <t>Poly(thiophene-alt-ethylene glycol)</t>
         </is>
       </c>
     </row>
@@ -4384,7 +4386,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>Polypyrrole doped with dodecylbenzenesulfonate (Ppy:DBS);</t>
+          <t>Ppy:DBS</t>
         </is>
       </c>
     </row>
@@ -4414,7 +4416,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>EuroPN-VM; DNAs; (BEDT-TTF)2(ReO4); (BEDT-TTF)2(ReO4); (TTF)2F(So3)</t>
         </is>
       </c>
     </row>
@@ -4424,7 +4426,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>P3HT-DPA; Poly(thiophene); Poly(thiophene-2,5-diyl)</t>
+          <t>Thiophene-based trimer; Dipicolylamine-modified conducting polymer</t>
         </is>
       </c>
     </row>
@@ -4434,7 +4436,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>Lignosulfonate; Partially desulfonated lignosulfonate; Lignin</t>
+          <t>Lignosulfonate; partially desulfonated lignosulfonate; fully desulfonated lignin</t>
         </is>
       </c>
     </row>
@@ -4444,7 +4446,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>EDO-TTF-SCN; β''-Fermionene; (PTTP)[Ag(CN)2]; (PTTP)[DMF-PF6]</t>
+          <t>PEDT-PSS; PNDI-TN; DN-TN; F4TCNQ; TCNQ</t>
         </is>
       </c>
     </row>
@@ -4464,7 +4466,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>Polymers; None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4474,7 +4476,7 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>CH(NH2)(2)PbBr3; CH3NH3PbBr3; CH3NH3PbI3</t>
         </is>
       </c>
     </row>
@@ -4484,7 +4486,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>spiro-NDI-N</t>
+          <t>spiro-NDI-N;</t>
         </is>
       </c>
     </row>
@@ -4494,7 +4496,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate) (PEDOT:PSS); P3HT-TTP; P3HT-Thienyl-TTP; Poly[2-methoxy-5-(2'-ethylhexyloxy)-1,4-phenylenevinylene] (MEH-PPV)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4504,7 +4506,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>(BEDT-TTF)Cl; (CMeTCNQ)</t>
+          <t>(BEDT-TTF)ClMeTCNQ;</t>
         </is>
       </c>
     </row>
@@ -4514,7 +4516,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>TTF-TCNQ-LiTFSI-H2O</t>
+          <t>TTF-TCNQ; LiTFSI</t>
         </is>
       </c>
     </row>
@@ -4544,7 +4546,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>Pedot:Pss</t>
+          <t>PEDOT:PSS; SO3H-Si-MCM-41; Poly(3,4-ethylenedioxythiophene)</t>
         </is>
       </c>
     </row>
@@ -4564,7 +4566,7 @@
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>(BEDO-TTF)(Cl(2)TCNQ)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4574,7 +4576,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>PTAA; Poly(3,4-ethylenedioxythiophene) (PEDOT); Spiro-MeOTAD; Poly(2-methoxy-5-(2'-ethyl-hexyloxy)-1,4-phenylenevinylene) (MEH-PPV); Poly-(9,9-dioctylfluorene-alt-4-methyloxynaphthalene-ethenylene-alt-6-isoynapthylene-ethyl-3,6-dioctyl-benzocryptene) (Poly-PF); Poly(3-hexylthiophene-2,5-diyl) (P3HT)</t>
+          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3,4-ethylenedioxythiophene)-silica; Poly(3,4-propylenedioxythiophene); Polypyrrole; Polythiophene Blend</t>
         </is>
       </c>
     </row>
@@ -4604,7 +4606,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>Poly(anthraquinonyl-imide); Poly(indole-5-carboxamide); None</t>
+          <t>Poly(ethylene oxide)-containing polymer; Solvatochromic Naphthalimide-based OMIEC</t>
         </is>
       </c>
     </row>
@@ -4614,7 +4616,7 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; Poly(3,4-ethylenedioxythiophene) (PEDOT); Polypyrrole; Poly(3-hexylthiophene) (P3HT)</t>
+          <t>P(3-octylphenol thiosemicarbazone), poly(3,4-ethylenedioxythiophene), Conducting Polymer of Pyrrole Co-Polymerized with Neutral Red</t>
         </is>
       </c>
     </row>
@@ -4634,7 +4636,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)-TCNQ; Poly(indole-5-carboxylic acid)-DCNQI; None</t>
+          <t>Poly(ethylene-alt-TCNQ); Poly(ethylene-alt-DCNQI); [Ru-2(II,II)(dcnqi)(2)]; None</t>
         </is>
       </c>
     </row>
@@ -4644,7 +4646,7 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>Polyvinylpyrrolidone-Poly(3-hydroxybenzoic acid) Bithiophene; Poly(3,4-ethylenedioxythiophene)-Poly(ethylene oxide); Poly(3,4-ethylenedioxythiophene)-Poly(styrenesulfonate); None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4654,7 +4656,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>PM6;</t>
+          <t>PM6;CH1007</t>
         </is>
       </c>
     </row>
@@ -4664,7 +4666,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(triphenylamine) (PTPA); Poly(fluorene); Poly(vinylidene fluoride-hexafluoropropylene) (PVDF-HFP)</t>
+          <t>PEDOT:PSS; Poly(3,4-ethylenedioxythiophene); poly(ethylene oxide)-based complex polymer electrical conductors</t>
         </is>
       </c>
     </row>
@@ -4674,7 +4676,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>[C6MIM][PF6];</t>
         </is>
       </c>
     </row>
@@ -4684,7 +4686,7 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>Poly(ethylene oxide)-BMIMBF4; Poly(vinylidene fluoride-co-hexafluoropropylene)-BMIMBF4</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4694,7 +4696,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>PEDOT:PSS;</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -4704,7 +4706,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>PEDOT-PSS; P3MT; PMMA-PPO; PPy/PVAc; PPy; PBTTT-CF3; Poly(3,4-ethylenedioxythiophene)-sodium; None</t>
+          <t>Poly(ethylene oxide)-based OMIEC; Poly(o-methoxy aniline)-based OMIEC; Poly(3,4-ethylene dioxythiophene) (PEDOT) based OMIEC; Poly(quinoline) based OMIEC; Poly(thiophene) based OMIEC</t>
         </is>
       </c>
     </row>
@@ -4714,7 +4716,7 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>Polymer;poly(styrene-alt-maleic anhydride);polypyrrole;PEDOT-PSS</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4724,7 +4726,7 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>PEO; poly(ethylene glycol) 3400</t>
+          <t>PEO; Li-x(MoS2)(polyether)(y)</t>
         </is>
       </c>
     </row>
@@ -4734,7 +4736,8 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>Poly(3-hydroxythiophene-bisurea); Poly(3,4-ethylenedioxythiophene-bisurea); Poly(N-vinyl-benzidine); Poly(fluorene-co-thiophene-bisurea); Poly(thiophene-co-furan)-alt-phenylene vinylene</t>
+          <t>Polymer; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-alkylthiophene) (P3AT); Poly(fluorene) (PF); Poly(phenylene vinylene) (PPV); 
+(Note: The output polymers are the ones mentioned in the text that belong to the OMIEC class, without repeating any names and without including 'OMIEC' or 'OMIEC based' in the output.)</t>
         </is>
       </c>
     </row>
@@ -4744,7 +4747,7 @@
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylene dioxythiophene) (PEDOT); Poly(3,4-ethylenedioxythiophene)-poly(4-styrenesulfonate) (PEDOT-PSS); Poly(2-methoxy,5-hexyloxyphenylene vinylene) (PV-OPV); Poly(3-hexylthiophene) (P3HT)</t>
+          <t>Dendrimer-Cu2(C6H5COO)2; Poly(3,4-ethylene dioxythiophene)-poly(styrenesulfonate)</t>
         </is>
       </c>
     </row>
@@ -4774,7 +4777,7 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>PVDF-HFP;</t>
         </is>
       </c>
     </row>
@@ -4814,7 +4817,7 @@
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>PEOEIPT; P3HT; PEDOT:PSS; poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); poly(triarylamine)</t>
+          <t>CH3NH3PbI3</t>
         </is>
       </c>
     </row>
@@ -4844,7 +4847,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>PTh-Cp*; PAni-Cp*; PPy-Cp*</t>
+          <t>PPy; PTh; PAni</t>
         </is>
       </c>
     </row>
@@ -4854,7 +4857,7 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>Polymers found: Polyaniline-Polyvinylpyrrolidone; Polythiophene-Polyvinylpyrrolidone; Polypyrrole-Polyvinylpyrrolidone; Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); Poly(3,4-ethylenedioxythiophene)-poly(ethylene oxide); Poly(acrylonitrile-co-maleic acid)-polyvinylpyrrolidone; None</t>
+          <t>PQTSA; 2,4,4-Trimethylpentane-2-tert-Butylphenol Polymers; Perylene-3,4-dicarboximide; Perylenetetracarboxylic diimide; PTAA; PTEC; PBTT; PBTT-HT; PFBTT; BPEPED-T; BPEPED-H; BPEPED-; PEI-PDMS; PEI-PTMC; PEI-P4VP; PEO-Poly(Aspartic acid); PEO-Poly(Lysine); PBTT-T; PBTT-D; PFO; PSBT</t>
         </is>
       </c>
     </row>
@@ -4874,7 +4877,7 @@
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>Polymeric ion gel; PEDOT:PSS; Polypyrrole; Poly(3,4-ethylenedioxythiophene)</t>
+          <t>Polymer;</t>
         </is>
       </c>
     </row>
@@ -4884,7 +4887,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene):polystyrenesulfonate; Polyacrylamide-Phenylboronic Acid Gel</t>
+          <t>poly(3,4-ethylenedioxythiophene):polystyrenesulfonate;</t>
         </is>
       </c>
     </row>
@@ -4894,7 +4897,7 @@
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>PTCDA; PTCBI; PTCDI</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4904,7 +4907,7 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>Polyaniline; Polypyrrole</t>
+          <t>no OMIEC polymers mentioned</t>
         </is>
       </c>
     </row>
@@ -4924,7 +4927,7 @@
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>Poly[4-styryl-1,2,5-benzothadiazole]; Poly[2-methoxy-5-(2'-ethylhexyloxy)-1,4-phenylenevinylene]; Poly(3,4-ethylenedioxythiophene); Poly(3-methylthiophene)</t>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -4954,7 +4957,7 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>PNNM;Poly(thiophene-3-acetic acid);Poly(phenylvinylene);Poly(pyridine-2-yl-aldimine-3'-ylimine);Poly(perylenediimide)</t>
+          <t>(BuG)(F(n)TCNQ)</t>
         </is>
       </c>
     </row>
@@ -4964,7 +4967,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(N-vinylcarbazole); Poly(phenylene vinegar) (PPV); Polyaniline (PANI); Polythiophene (PT); Poly(2-methoxy-5-(2´-ethylhexyloxy)-1,4-phenylene vinylene) (MEH-PPV); Poly(3-hexylthiophene) (P3HT).</t>
+          <t>Poly(aniline-co-o-toluidine); Poly(ethylene dioxythiopene); Poly(3,4-ethylenedioxythiophene); Polyphenylamine; Poly(thieno[3,4-b]thiophene); Poly(methylphenylsilyl-3,4-ethylenedioxythiophene); None</t>
         </is>
       </c>
     </row>
@@ -4974,7 +4977,7 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>La2NiO4;</t>
+          <t>L2NO4None</t>
         </is>
       </c>
     </row>
@@ -4994,7 +4997,7 @@
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>PIM-HQNA;PITQ-SIPQ;PEO-TFSI;PSSH;PSeSC;PTA-DMF</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5004,7 +5007,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>CPE-K; slow-evaporation-water-soluble-CPE</t>
+          <t>CPE-K</t>
         </is>
       </c>
     </row>
@@ -5024,7 +5027,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) - poly(styrenesulfonate); Poly(3-dodecylthiophene); Poly(9,9-dioctylfluorene-alt-4,7-bis(thiophen-2-yl)benzo[c][1,2,5]thiolazine); None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5044,7 +5047,7 @@
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; P3HT; PQT; PTAA</t>
+          <t>C60/Organic Self-Assembled Monolayer</t>
         </is>
       </c>
     </row>
@@ -5054,7 +5057,7 @@
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>Vanadylphthalocyanine porphyrazine; Vanadyltetralds(1,2,S-thiadiazole)porphyrazine</t>
+          <t>VOPc; vanadyltetralds(1,2,S-thiadiazole)porphyrazine</t>
         </is>
       </c>
     </row>
@@ -5074,7 +5077,7 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>PolyNDI-BTBT; PNPB; poly(3,4-ethylenedioxythiophene)-poly(4-styrenesulfonate); Poly(3-hexylthiophene)-poly(ethylene oxide); Poly(chloroaluminophosphonate)-poly(methylpyrrole)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5084,7 +5087,7 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>Poly(ethylene oxide)-based polymer electrolyte; Poly(vinylidene fluoride)-based polymer electrolyte; Nafion; Poly( methyl methacrylate)-based polymer electrolyte; Poly(ethylene oxide) -b- Poly(butylene oxide); PEDOT-PSS</t>
+          <t>PMDI-30; PMEI-30; PMMA-Imide-PEI; Polymidine-PEO; Polypyrrole-PEO; Poly(alkylimidazolium) ionic liquids; EDOT-TTF.</t>
         </is>
       </c>
     </row>
@@ -5114,7 +5117,7 @@
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); Poly(bis-(3-methylcarbazole)-alt-2,7-(9,9-di-n-octyl-9H-fluoren-2-yl)-fluorene)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5124,7 +5127,7 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)-polystyrenesulfonate; poly(2-methoxy-5-(2'-ethylhexyloxy)-p-phenylenevinylene)-tetrathiafulvalene; none</t>
+          <t>Poly(3,4-ethylenedioxythiophene):poly(styrenesulfonate); Poly(3-hexylthiophene)</t>
         </is>
       </c>
     </row>
@@ -5134,7 +5137,7 @@
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MAI; FAI</t>
         </is>
       </c>
     </row>
@@ -5194,7 +5197,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>Bithiophene-Thienothiophene Conjugated Polymer; Propylene-Based Conjugated Polymer; Butylene-Based Conjugated Polymer</t>
+          <t>Bithiophene-thienothiophene polymer; poly(ethylene glycol bithiophene-thienothiophene); poly(propylene bithiophene-thienothiophene); poly(butylene bithiophene-thienothiophene)</t>
         </is>
       </c>
     </row>
@@ -5204,7 +5207,7 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>Eumelanin</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5234,7 +5237,7 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)</t>
+          <t>poly(3,4-ethylenedioxythiophene);</t>
         </is>
       </c>
     </row>
@@ -5244,7 +5247,7 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>No OMIEC polymer was found.</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5254,7 +5257,7 @@
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; Poly(3,4-ethylenedioxythiophene); Poly(phenylene ethynylene); Polyurethane-Graft-Poly(3,4-ethylenedioxythiophene); Poly(3-hexylthiophene)</t>
+          <t>Polymer electrodes; PEDOT:PSS; PPy; PANI</t>
         </is>
       </c>
     </row>
@@ -5274,7 +5277,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>PTMA; PBI-NH3+; unknown</t>
+          <t>PTMA</t>
         </is>
       </c>
     </row>
@@ -5284,7 +5287,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Polymer ; None</t>
         </is>
       </c>
     </row>
@@ -5304,7 +5307,7 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>P3HT; PPE; PEDOT; PSS; PTh; PPV</t>
+          <t>PEDOTP;</t>
         </is>
       </c>
     </row>
@@ -5314,7 +5317,7 @@
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>poly-N,phenylene-vinylene; PEDOT:PSS; P3HT; PTAA</t>
+          <t>Polymer(s): PECDA;</t>
         </is>
       </c>
     </row>
@@ -5324,7 +5327,7 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>Poly[Ni(CH3Osalen)]</t>
+          <t>poly[Ni(CH3Osalen)];</t>
         </is>
       </c>
     </row>
@@ -5344,7 +5347,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>TTF-CA; Radical-PNN; Alkali-TCNQ</t>
+          <t>TTF-CA; METAL COMPLEXES; ALKALI-TCNQ; SrTiO3</t>
         </is>
       </c>
     </row>
@@ -5364,7 +5367,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>PEO</t>
+          <t>Poly(oxyethylene) (PEO)-based polymer; NASICON-type ionic conductor covered with the PEO-based polymer</t>
         </is>
       </c>
     </row>
@@ -5424,7 +5427,7 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>PolymerElectrolyte; Poly(9,9-dioctylfluorene-co-N,N'-bis(4-butyl-phenyl)-N,N'-bis(phenyl)-1,4-phenylenediamine); Spiro[fluorene-alt-benzothiadiazole]; Poly(9,9-dioctyl-3,6-bis(N-carbazolyl)-2,7-diyl)(EMA-3.4)</t>
+          <t>Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); Poly(9,9-di-n-octylfluorene)-Poly(styrenesulfonate); PEDOT-PSS; PSS; Fluorene-PSS</t>
         </is>
       </c>
     </row>
@@ -5464,7 +5467,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>Poly(ethylene oxide); Di-iso-propyl ammonium tetracyano-p-quinodimethanide (PDS); Di-butylammonium tetracyano-p-quinodimethanide (DBA); Di-sec-butylammonium tetracyano-p-quinodimethanide (DSBA)</t>
+          <t>Poly(ethylene oxide)</t>
         </is>
       </c>
     </row>
@@ -5474,7 +5477,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>PEDOT/PSS; Poly(2,2'-bithiophene)-alt-5,5'-diethyl-2,2'-bithiazole; Poly(2,7-carbazole-alt-5,5'-di(2-thienyl)-2,2'-bithiazole); Poly(3-alkoxy-4-methylthiophene); Poly(3-ethoxy-4-methylthiophene); None</t>
+          <t>Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); Poly(3,4-ethylenedioxythiophene)-co-poly(3,4-ethylenedioxythiophene); P3HT-TTF; P3HT-CuPc; P3HT-OFET; P3HT-tribenzotetraazaporphyrin; P3HT-Perfluoro-2,5-diyl-benzene</t>
         </is>
       </c>
     </row>
@@ -5484,7 +5487,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>Cellulose-based organic mixed ionic electronic conductor;</t>
+          <t>Cellulose; OrganoiCE</t>
         </is>
       </c>
     </row>
@@ -5504,7 +5507,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; PBTTT-DPP; P3HT; PPy; PIVAC</t>
+          <t>Polyindenofluorene; Poly(3,4-ethylenedioxythiophene)-poly(4-styrenesulfonate); None</t>
         </is>
       </c>
     </row>
@@ -5524,7 +5527,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>CuHCF; Prussian Blue Analogue (PBA)</t>
+          <t>Prussian Blue Analogue (PBA); CuHCF; NiHCF; CoHCF</t>
         </is>
       </c>
     </row>
@@ -5534,7 +5537,7 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Poly(2-(benzo[d]thiazol-2-yl)-9-ethyl-9H-carbazol); Poly(9-ethyl-9H-carbazol-2-yl)-1,3-benzothiazole; None</t>
         </is>
       </c>
     </row>
@@ -5544,7 +5547,7 @@
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>MA; FA; none</t>
+          <t>MA; FA</t>
         </is>
       </c>
     </row>
@@ -5554,7 +5557,7 @@
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>Poly[2-methoxy-5-(2'-ethylhexyloxy)-1,4-phenylene vinylene]; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(thiophene-3-carboxylic acid); Poly(p-phenylene vinylene); Poly(3-hexylthiophene) (P3HT)</t>
+          <t xml:space="preserve"> PEDOT; P3HT; Poly(3,4-ethylenedioxythiophene); None</t>
         </is>
       </c>
     </row>
@@ -5564,7 +5567,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>poly(phenylene vinylene); PEDOT-PSS</t>
+          <t>conducting polymers;</t>
         </is>
       </c>
     </row>
@@ -5584,7 +5587,7 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>Cytosine-MeTCNQ;</t>
+          <t>MeTCNQ</t>
         </is>
       </c>
     </row>
@@ -5594,7 +5597,7 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>Polythiophene-graft-poly(caprolactone-block-dimethylaminoethyl methacrylate); Polythiophene-g-PCL-b-PDMAEMA</t>
+          <t>Polythiophene-graft-poly(caprolactone-block-dimethylaminoethyl methacrylate)</t>
         </is>
       </c>
     </row>
@@ -5604,7 +5607,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>1-octyl-3-methylimidazolium chloride; 1-octyl-3-methylimidazolium hydrogen sulphate; 1-butyl-3-methylimidazolium hydrogen sulphate</t>
+          <t>1-octyl-3-methylimidazolium hydrogen sulphate; 1-butyl-3-methylimidazolium hydrogen sulphate; 1-butyl-3-methylimidazolium bromide;</t>
         </is>
       </c>
     </row>
@@ -5614,7 +5617,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>P(ProDOT)s</t>
+          <t>P(ProDOT)</t>
         </is>
       </c>
     </row>
@@ -5624,7 +5627,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>poly(2-carboxyphenylhydroquinone-alt-4-methyl-N-vinylpyridinium methoxysulfonate);</t>
+          <t>2-CPHMN</t>
         </is>
       </c>
     </row>
@@ -5634,7 +5637,7 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>p(g3T2)</t>
+          <t>p(g3T2);</t>
         </is>
       </c>
     </row>
@@ -5664,7 +5667,7 @@
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>PEDOT:PSS;</t>
+          <t>PEDOT:PSS; PANI</t>
         </is>
       </c>
     </row>
@@ -5674,7 +5677,7 @@
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>Poly(p-phenylene vinylene)-nickel oxide; Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate)-nickel oxide</t>
+          <t>(La,Sr)CoO3</t>
         </is>
       </c>
     </row>
@@ -5704,7 +5707,7 @@
       </c>
       <c r="B527" t="inlineStr">
         <is>
-          <t>P3TAA-VOMe; PT-CPT-I-PBI-DY; PT-PBI-NH3+; P3TAA-ran-P3HT-MAPbI3; APT; PT-g-(PDMAEMA-co-PGLU-HEM)</t>
+          <t>P3TAA; CPT-I-PBI-DY; PBI-NH3+-PT</t>
         </is>
       </c>
     </row>
@@ -5714,7 +5717,7 @@
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>PMDT-TTF; P3HT-TFE; PFPV-TPMV; Naphthalene-Tetracyanoethylene; F4TCNQ-TTNF; TTNF-TCNQ</t>
+          <t>PMDI;PBTM;PCEME</t>
         </is>
       </c>
     </row>
@@ -5754,7 +5757,7 @@
       </c>
       <c r="B532" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>tTTF-I</t>
         </is>
       </c>
     </row>
@@ -5814,7 +5817,7 @@
       </c>
       <c r="B538" t="inlineStr">
         <is>
-          <t>MP-TTF(2,5-difluoro-TCNQ); MP-TTF(2,5-dimethyl-TCNQ); MP-TTF(2-methoxy-5-ethoxy-TCNQ); MP-TTF(fluoro-TCNQ); MP-TTF(TCNQ); MP-TTF(decyl-TCNQ)</t>
+          <t>MP-TTF-2,5-difluoro-TCNQ; MP-TTF-fluoro-TCNQ; MP-TTF-TCNQ; MP-TTF-decyl-TCNQ; MP-TTF-2,5-dimethyl-TCNQ; MP-TTF-2-methoxy-5-ethoxy-TCNQ</t>
         </is>
       </c>
     </row>
@@ -5824,7 +5827,7 @@
       </c>
       <c r="B539" t="inlineStr">
         <is>
-          <t>PSS; PDAC</t>
+          <t>Sodium poly(styrene sulfonic acid); poly(diallyl dimethylammonium chloride)</t>
         </is>
       </c>
     </row>
@@ -5834,7 +5837,7 @@
       </c>
       <c r="B540" t="inlineStr">
         <is>
-          <t>P2VP-Pt; P3HT-DMF; P3HT-TMC; PFN-PEDOT-PSS; PEDOT-PSS-Cu; PEDOT-PSS-CuI; PEDOT-PSS-PEO; PEDOT-PSS-PTP; PEO-PMMA; PEO-PPO-PEO; PPY-PSS; PSS-HAP; PSS-PVDF; PSS-PVP; PVC-PVP; PTBP-Py; PTCT-PVOH</t>
+          <t>Polymer; PPy; PFO-Th; F8BT; F8T2; F8; HTM</t>
         </is>
       </c>
     </row>
@@ -5844,7 +5847,7 @@
       </c>
       <c r="B541" t="inlineStr">
         <is>
-          <t>Poly(vinylbenzyltrimethylammonium) fluoride; Poly(ethylene oxide)-based membrane; PEO-based OMIEC polymer; None</t>
+          <t>Polymerized-Ionic Liquid-Organic Mixed Electronic Conductor; Polymeric and Organic/Inorganic Hybrid Membranes</t>
         </is>
       </c>
     </row>
@@ -5854,7 +5857,7 @@
       </c>
       <c r="B542" t="inlineStr">
         <is>
-          <t>P3HT;</t>
+          <t>RRa P3HT</t>
         </is>
       </c>
     </row>
@@ -5864,7 +5867,7 @@
       </c>
       <c r="B543" t="inlineStr">
         <is>
-          <t>Polymersemiconductors; Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); Poly(3-hexylthiophene); None</t>
+          <t>Fused thienosilinequinon;squaraine;quinoxaline derivatives;polyfluorene;polyphenylvinylene;poly(p-phenylene vinylene);poly(2,5-diketopyrrolopyrrole);poly(3,6-carbazole); poly(tetrafluoroethylene-alt-2,5-dibromo-1,4-phenylenevinylene)</t>
         </is>
       </c>
     </row>
@@ -5884,7 +5887,7 @@
       </c>
       <c r="B545" t="inlineStr">
         <is>
-          <t>PTCDI-PDMOT-TTF; MEH-PPV-TCNQ; N,N'-Bis(3-methyl-4-ethoxycarbonylphenyl)-perylene-3,4-dicarboximide-acceptor molecules-TCNQ-donor molecules</t>
+          <t>PTMA-TCNQ; Foley's salt; α-(NNN'-DMET-TTF)2Cr53+; poly(EDA-TTF)</t>
         </is>
       </c>
     </row>
@@ -5904,7 +5907,7 @@
       </c>
       <c r="B547" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-hexylthiophene) (P3HT); Eurion; Poly[[9,9-bis(3'-(N,N-dimethylamino)propyl)-2,7-(carbazole)]]; None</t>
         </is>
       </c>
     </row>
@@ -5984,7 +5987,7 @@
       </c>
       <c r="B555" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2,9-bis(N-decylaminocarbonyl)-1,10-phenanthroline;</t>
         </is>
       </c>
     </row>
@@ -5994,7 +5997,7 @@
       </c>
       <c r="B556" t="inlineStr">
         <is>
-          <t>PEDOT-PSS; P3HT-TFSA; Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate); Poly(3-dodecylthiophene)-poly(styrenesulfonate); poly-thiophene-PF6; None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6004,7 +6007,7 @@
       </c>
       <c r="B557" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; P3HT/PEDOT:PSS; CoPc-PEDOT:PSS; C60-PEDOT:PSS</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -6014,7 +6017,7 @@
       </c>
       <c r="B558" t="inlineStr">
         <is>
-          <t>Spiro-(1,1')-bipyrrolidinium tetrafluoroborate (SBPBF4);</t>
+          <t>Spiro-(1,1')-bipyrrolidinium tetrafluoroborate;</t>
         </is>
       </c>
     </row>
@@ -6054,7 +6057,7 @@
       </c>
       <c r="B562" t="inlineStr">
         <is>
-          <t>PEO-PVDF-Hf(HCOO)2; P(VDF-TrFE)/KOH; PEO-PVDF-In(I)(COO)2; PEDOT:PSS/RuOx; PEDOT:PSS/TaOx; PEO-PVDF-Al(HCOO)2</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6084,7 +6087,7 @@
       </c>
       <c r="B565" t="inlineStr">
         <is>
-          <t>PMDIT; PADIIP; Poly(3,4-ethylenedioxythiophene)-block-Poly(styrenesulfonate) (PEDOT-PSS); PEDOT-PPy-PSS; N,N'-Bis(4-(thien-3-yl)phen-2-ylmethylene)bis(N-benzyl-3-methoxybenzamide) (TAA-TBMA); N,N'-Bis(4-(pyrrol-3-yl)phen-2-ylmethylene)bis(N-benzyl-3-methoxybenzamide) (PAA-TBMA)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6094,7 +6097,7 @@
       </c>
       <c r="B566" t="inlineStr">
         <is>
-          <t>PEDOT:PSS; PPy; PPV; F8T2; F16CuPc; Nafion; poly(ethylene oxide); Poly(3-methylthiophene); BPEI</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6104,7 +6107,7 @@
       </c>
       <c r="B567" t="inlineStr">
         <is>
-          <t>Polyvinyl-benzyl-3-methylimidazolium tetrafluoroborate; Polyvinyl-benzyl-3-methylimidazolium hexafluorophosphate; Poly(3-methylimidazolium chloride); Poly(ethylene oxide-block-poly(butadiene-b-ethylene oxide)) containing ionic liquid moieties; None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6124,7 +6127,7 @@
       </c>
       <c r="B569" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Polymer names (separated by semicolons) mentioned in the text are: Mg2Al-vinyl benzene sulfonate (VBS)</t>
         </is>
       </c>
     </row>
@@ -6144,7 +6147,7 @@
       </c>
       <c r="B571" t="inlineStr">
         <is>
-          <t>PTCDA;  poly(3,4-ethylene dioxythiophene);  poly(3-methylthiophene);  poly[N-(2-(thien-5-yl)ethen-1-yl)-4-methylthieno[3,4-b][dithiophene);  poly(triarylamine);  poly(N,N'-dialkyl-3,4,9,10-perylenetetracarboxylic diimide);</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6164,7 +6167,8 @@
       </c>
       <c r="B573" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxi-theno)[3,4-c]pyrrole-4,7-phthalazine (PEDT-PPT); PTV[6]-BT; PPy-PTh; PANI-PTh; PVT[6]-BTT</t>
+          <t>I found some OMIEC polymers, but there's only one:
+L-α-phosphatidylcholine; Cholesterol/phospholipidmixed vesicles</t>
         </is>
       </c>
     </row>
@@ -6174,7 +6178,7 @@
       </c>
       <c r="B574" t="inlineStr">
         <is>
-          <t>PSePPT; PEDOT:PSS</t>
+          <t>Polymer; Poly(N-vinyl-2-pyrrolidone)-based (PVP); PEDOT-PSS (Poly(3,4-ethylenedioxythiophene)-poly(4-styrenesulfonate)); Poly(3-hexylthiophene) (P3HT); Poly(3-butylthiophene) (PBUT); Poly(3-octylthiophene) (POT); Poly(indole-2-carboxylic acid-co-7-(2'-thienyl)-indole) (P(II); Poly(3,4-ethylenedioxythiophene)-poly styreme sulfonate) (PEDOT/PSS); Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(phenylene vinylene); Polyaniline (PANI); Poly-o-phenylenediamine); Polythiophene; Polypyrrole (PPy); Poly(cephalosporinomethyl-co-2-(bis(1,1-dimethyl) propane-1,3-diyl)oxy)ethyl)-3-(1,1-dimethyl) propane-3-yl)oxy)ethoxy)ethoxy)ethoxy)ethoxy); Poly(cephalosporinomethyl-co-2-(bis(1,1-dimethyl) propane-1,3-diyl)oxy)ethyl)-3-(1,1-dimethyl) propane-3-yl)oxy)ethoxy)ethoxy)ethoxy)ethoxy);</t>
         </is>
       </c>
     </row>
@@ -6184,7 +6188,7 @@
       </c>
       <c r="B575" t="inlineStr">
         <is>
-          <t>PMDI; PTAA; PTAA-MeI; DCHDIT(Tos); TPBi; Spiro-OMeTAD; PTCDA</t>
+          <t>Poly[phe-nyl-C3NH2Li(SeCN)2]+; Poly[bis(ethylenedioxylthiopyranyl)imide]; Poly[bis(3-propyl-1H-pyrrole-1-carbonyl)sulfone]; Poly[oxy-3-fluorophenyl-3-fluorophenyl-COO-3-fluorophenyl-3-fluorophenyl-COO]; Poly[3-methyl-N-(3-pyridyl)pyrrole-2,5-diyl]; Poly[5-[(1,3-bis(2-ethylhexyl)-1,1,3,3-tetramethylindolyl)-methyl]-2,2'-bithiophen-5-yl-yl]; Poly(o-tolunitrile); Poly(N-vinylcarbazole); Poly(3-phenyl-[1,2,5]thiadiazol-(3,4-c)-thiophen);</t>
         </is>
       </c>
     </row>
@@ -6204,7 +6208,7 @@
       </c>
       <c r="B577" t="inlineStr">
         <is>
-          <t>PETTIFUL; PIMCOB; PIDTCE; PEOPT; PEDOT-PSS</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6214,7 +6218,7 @@
       </c>
       <c r="B578" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Polymer; Cocrystal; none</t>
         </is>
       </c>
     </row>
@@ -6264,7 +6268,7 @@
       </c>
       <c r="B583" t="inlineStr">
         <is>
-          <t>Poly(4-(2-chloroanilino)-1,3-butadiene-2-one); Poly(pyridine-2-carboxaldehyde-4-methoxybenzylideneaminohydrazide); None</t>
+          <t>Poly(4-3-(hydroxyimino)-4-oxopentan-2-ylidene)amino)-1,5-dimethyl-2-phenyl-1H-pyrazol-3(2H)-one; Polypyrazolone-mercury(II) complex; Polypyrazolone-cobalt(II) complex; Polypyrazolone-manganese(II) complex; Polypyrazolone-zinc(II) complex</t>
         </is>
       </c>
     </row>
@@ -6284,7 +6288,7 @@
       </c>
       <c r="B585" t="inlineStr">
         <is>
-          <t>PTAA; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(phenylene oxide) (PPO); Poly(phenylene sulfide) (PPS); Poly(styrenesulfonate) (PSS); Poly(2-methoxy-5-(2'-ethylhexyloxy)-p-phenylenevinylene) (MEH-PPV);  ITO-PEG;  P3HT-PEO; PCE-PEO</t>
+          <t>imidazole based coatings</t>
         </is>
       </c>
     </row>
@@ -6304,7 +6308,7 @@
       </c>
       <c r="B587" t="inlineStr">
         <is>
-          <t>(BEDO-TTF)2(CF3TCNQ); (TMTSF)2(CF3TCNQ); Tetramethyl-TTF·CF3TCN·CH3CN; Bis(methylthio)ethylenedithio-TTF·CF3TCN</t>
+          <t>Bedo-TTF; bis(methylthio)ethylenedithio-TTF; tetramethyl-TTF</t>
         </is>
       </c>
     </row>
@@ -6344,7 +6348,7 @@
       </c>
       <c r="B591" t="inlineStr">
         <is>
-          <t>Poly(3-hexylthiophene)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6354,7 +6358,7 @@
       </c>
       <c r="B592" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>PA6 (polyamide 6)</t>
         </is>
       </c>
     </row>
@@ -6374,7 +6378,7 @@
       </c>
       <c r="B594" t="inlineStr">
         <is>
-          <t>P-[6-12-6]-OMe; P-[12]-OMe; P-[6-12-6][-SiMe3Ph]; P-[6]-OMe; P-[12]-OMe[-SiMe3Ph]; P-[12][-SiMe3Ph][6][-SiMe3Ph]</t>
+          <t>[6-12-6]</t>
         </is>
       </c>
     </row>
@@ -6434,7 +6438,7 @@
       </c>
       <c r="B600" t="inlineStr">
         <is>
-          <t>PPEO; PDBS; PEO-Tr-BTZ; PEO-Tr-TTF; P3HT-DBSA; PTAA; PEDOT-PSS; PTTP; P3OT-DBSA; PFTT; PEI-DNA; PEO-DBSA</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6454,7 +6458,7 @@
       </c>
       <c r="B602" t="inlineStr">
         <is>
-          <t>Naphthalene-1,4,5,8-tetracarboxylic-diimide-bithiophene;</t>
+          <t>Naphthalene-1,4,5,8-tetracarboxylic-diimide-bithiophene</t>
         </is>
       </c>
     </row>
@@ -6464,7 +6468,7 @@
       </c>
       <c r="B603" t="inlineStr">
         <is>
-          <t>P3HT</t>
+          <t>P3HT;</t>
         </is>
       </c>
     </row>
@@ -6484,7 +6488,7 @@
       </c>
       <c r="B605" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-methylthiophene); Poly(3-thiophene acetic acid); Poly(9,9-dioctylfluorene-co-benzothiadiazole); Poly(3,4-ethylenedioxythiophene)-block-poly(ethylene oxide); Poly(thiophene- vinylene); Poly(3-thiophene ethylamine); Poly(3-thiophene acrylate); Poly(3,4-dimethoxythiophene); None</t>
+          <t>Poly(p-phenylenevinylene)-coated poly(ethylene oxide); poly(3,4-ethylenedioxythiophene)-coated poly(ethylene oxide); poly(aniline); poly(2-methoxy-5-(2-ethylhexyloxy)-1,4-phenylenevinylene)-coated poly(ethylene oxide); PEDOT:PSS; Polypyrrole:Poly(ethylene oxide); Conducting polymer-peptide conjugate</t>
         </is>
       </c>
     </row>
@@ -6494,7 +6498,7 @@
       </c>
       <c r="B606" t="inlineStr">
         <is>
-          <t>PEDOT:PSS-TTF; P3HT-TSF; PPP-TTF; FBu-PEDOT:TCNQ; ET-F4TCNQ; ESP-TTF; F4TCNQ-PPV; π-Conjugated Polymers; P3AT-TSF; ETMe4-CNQ.</t>
+          <t>Poly(p-phenylene vinylene) semiconducting polymers; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(aniline) (PANI); Poly(thiophene) derivatives; Poly(fluorene) derivatives; Poly(azomethine); PEDOT:PSS; PEDOT:PSS; Poly(3-hexylthiophene) (P3HT)</t>
         </is>
       </c>
     </row>
@@ -6504,7 +6508,7 @@
       </c>
       <c r="B607" t="inlineStr">
         <is>
-          <t>Polymer; Poly(3,4-ethylenedioxythiophene); Poly(thiophene);</t>
+          <t>Polymer networks; polythiophene</t>
         </is>
       </c>
     </row>
@@ -6524,7 +6528,7 @@
       </c>
       <c r="B609" t="inlineStr">
         <is>
-          <t>Polymer(s): Poly(3-hexylthiophene)-imidazolium (P3HT-I); (Poly(phenylenevinylene)-iminum) (PPV-I); Poly(3,4-ethylenedioxythiophene)-poly(styrenesulfonate) (PEDOT-PSS); Poly(aniline)-poly(styrenesulfonate) (PANI-PSS);</t>
+          <t>Dexamethasone; cortisol; prednisone</t>
         </is>
       </c>
     </row>
@@ -6534,7 +6538,7 @@
       </c>
       <c r="B610" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Polymer;Polymer;Polymer</t>
         </is>
       </c>
     </row>
@@ -6564,7 +6568,7 @@
       </c>
       <c r="B613" t="inlineStr">
         <is>
-          <t>Poly(N-isopropylacrylamide-co-oligo(ethylene glycol));</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6584,7 +6588,7 @@
       </c>
       <c r="B615" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>PEDOT:PSS</t>
         </is>
       </c>
     </row>
@@ -6594,7 +6598,7 @@
       </c>
       <c r="B616" t="inlineStr">
         <is>
-          <t>poly(VTPA-co-AMS);</t>
+          <t>poly(VTPA-co-AMS); TPB-crosslinked poly(VTPA-co-AMS)</t>
         </is>
       </c>
     </row>
@@ -6614,7 +6618,7 @@
       </c>
       <c r="B618" t="inlineStr">
         <is>
-          <t>PEDOT/PSS; PTS-Na</t>
+          <t>PTS-Na; PEDOT/PSS</t>
         </is>
       </c>
     </row>
@@ -6634,7 +6638,7 @@
       </c>
       <c r="B620" t="inlineStr">
         <is>
-          <t>PS-b-PLA; PS-b-PMMA</t>
+          <t>PS-b-PMMA; PS-b-PLA</t>
         </is>
       </c>
     </row>
@@ -6764,7 +6768,7 @@
       </c>
       <c r="B633" t="inlineStr">
         <is>
-          <t>PFBT-Th-PFBT; BTPF-Th-BT; BTPF-Th-PF; BTPF-Th-PFP; PFBT-Th-PFBT-BT; PFBT-Th-PFBT-Th-PF</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6794,7 +6798,7 @@
       </c>
       <c r="B636" t="inlineStr">
         <is>
-          <t>PPEIP; PEOPE; PFMPE; PEIO; PFMOP; PPEPO; PFMPE-F4T; PEOPE-F4T; PFMPEO-F4T</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6824,7 +6828,7 @@
       </c>
       <c r="B639" t="inlineStr">
         <is>
-          <t>PEDOT; P3T; EDOT-N-3 PTh2; Th3-TTh2; PTh3-TTh2</t>
+          <t>PEDOT/P3T; EDOT-N-3</t>
         </is>
       </c>
     </row>
@@ -6854,7 +6858,7 @@
       </c>
       <c r="B642" t="inlineStr">
         <is>
-          <t>PTTA; Poly(3,4-ethylenedioxythiophene) (PEDOT); Poly(3-hexylthiophene) (P3HT); Poly(3-methylthiophene) (PMTHT); None</t>
+          <t>DPP-TPA-BOD</t>
         </is>
       </c>
     </row>
@@ -7094,7 +7098,7 @@
       </c>
       <c r="B666" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)-based; Poly[2-methoxy-5-(2'-ethyl-hexyloxy)-p-phenylenevinylene]-based; Poly(thiophene-3-acetic acid)-based; Poly(9-(1-octyloxynonyl)-9H-carbazole)-based</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -7154,7 +7158,7 @@
       </c>
       <c r="B672" t="inlineStr">
         <is>
-          <t>PEO; PEO-TFBT; PEO-TMEMA; P3HT; PTB7; PTAA; PSS-COP; PSS-P3T; PSS-PdCAT; PS-b-P3HT</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -7164,7 +7168,7 @@
       </c>
       <c r="B673" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)-co-polystyrenesulfonate (PEDOT-PSS); Poly(4-styrenesulfonate)-co-poly(3-methylthiophene) (PSS-PTM); Poly(aniline-co-o-anisidine) (PANI/Poan); Poly(aniline-co-N-methyl aniline) (PANI/PNMA); Poly(thiophene-co-4,4'-bithiophene) (PTT/PBT); Poly(thiophene-co-3 methoxythiophene) (PTT/3-MT); Poly(4,4'-dithien-3,2'-pyrrole) (PDP); Poly(thiophene-co-2,5-dimethoxythiophene) (PTT/DMDT); Poly(3-hexylthiophene-co-3,4-ethylenedioxythiophene) (P3HT/PEDOT);</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -7274,7 +7278,7 @@
       </c>
       <c r="B684" t="inlineStr">
         <is>
-          <t>(Please input a text, I'll respond with the OMIEC polymers.)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -7474,7 +7478,7 @@
       </c>
       <c r="B704" t="inlineStr">
         <is>
-          <t>P3HT-OMIEC; PFO-OMIEC; PEDOT-OMIEC</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -8034,7 +8038,7 @@
       </c>
       <c r="B760" t="inlineStr">
         <is>
-          <t>PFBT; PBS; PEOIBT; PEO; PEDOT-PSS; PSSH; PANI-DBSA; PPy-VI; PEDOT-HT; F16CuPc; F8RuPc; PVDF-HFP</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -8234,7 +8238,7 @@
       </c>
       <c r="B780" t="inlineStr">
         <is>
-          <t>(R)-cAMPS; (S)-cAMPS</t>
+          <t>8-bromo-cAMP; 8-(4-chlorophenylthio)-cAMP; dibutyryl cAMP; (S-p)-5,6-DCl-cBiMPS; (S-p)-cAMPS</t>
         </is>
       </c>
     </row>
@@ -8364,7 +8368,7 @@
       </c>
       <c r="B793" t="inlineStr">
         <is>
-          <t>Poly(3,4-ethylenedioxythiophene)-co-poly(ethylene oxide); Poly(3,4-thiophene)-co-poly(ethylene oxide); Poly(ethylene oxide)-co-poly(aniline); None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -8404,8 +8408,7 @@
       </c>
       <c r="B797" t="inlineStr">
         <is>
-          <t>Polymer;Poly(3,4-ethylenedioxythiophene) (PEDOT);Poly[(9,9'-Bis(3-(3-ethyl-2-carboxy-vinyl)thiophen-2-yl)-9,9'-fluorenyl-2-carboxylate)-alt-(3,4-Ethylene dioxythiophene)]
-Note: I could only find a few OMIEC polymers mentioned in this text.</t>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>